<commit_message>
Added PEI,PR,SR,NR,TD,PO for DC1
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\James\DRP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5DE166-00C0-4859-A963-04AF875B28AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A22966-4266-4B17-9544-14E067FF1359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3363,15 +3363,6 @@
     <xf numFmtId="0" fontId="6" fillId="19" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3471,6 +3462,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7561,19 +7561,19 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="381" t="s">
+      <c r="C3" s="415" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="382"/>
-      <c r="E3" s="382"/>
-      <c r="F3" s="382"/>
-      <c r="G3" s="382"/>
-      <c r="H3" s="382"/>
-      <c r="I3" s="382"/>
-      <c r="J3" s="382"/>
-      <c r="K3" s="382"/>
-      <c r="L3" s="382"/>
-      <c r="M3" s="383"/>
+      <c r="D3" s="416"/>
+      <c r="E3" s="416"/>
+      <c r="F3" s="416"/>
+      <c r="G3" s="416"/>
+      <c r="H3" s="416"/>
+      <c r="I3" s="416"/>
+      <c r="J3" s="416"/>
+      <c r="K3" s="416"/>
+      <c r="L3" s="416"/>
+      <c r="M3" s="417"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
@@ -7945,19 +7945,19 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="381" t="s">
+      <c r="C4" s="415" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="382"/>
-      <c r="E4" s="382"/>
-      <c r="F4" s="382"/>
-      <c r="G4" s="382"/>
-      <c r="H4" s="382"/>
-      <c r="I4" s="382"/>
-      <c r="J4" s="382"/>
-      <c r="K4" s="382"/>
-      <c r="L4" s="382"/>
-      <c r="M4" s="383"/>
+      <c r="D4" s="416"/>
+      <c r="E4" s="416"/>
+      <c r="F4" s="416"/>
+      <c r="G4" s="416"/>
+      <c r="H4" s="416"/>
+      <c r="I4" s="416"/>
+      <c r="J4" s="416"/>
+      <c r="K4" s="416"/>
+      <c r="L4" s="416"/>
+      <c r="M4" s="417"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -8587,19 +8587,19 @@
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="381" t="s">
+      <c r="C23" s="415" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="382"/>
-      <c r="E23" s="382"/>
-      <c r="F23" s="382"/>
-      <c r="G23" s="382"/>
-      <c r="H23" s="382"/>
-      <c r="I23" s="382"/>
-      <c r="J23" s="382"/>
-      <c r="K23" s="382"/>
-      <c r="L23" s="382"/>
-      <c r="M23" s="383"/>
+      <c r="D23" s="416"/>
+      <c r="E23" s="416"/>
+      <c r="F23" s="416"/>
+      <c r="G23" s="416"/>
+      <c r="H23" s="416"/>
+      <c r="I23" s="416"/>
+      <c r="J23" s="416"/>
+      <c r="K23" s="416"/>
+      <c r="L23" s="416"/>
+      <c r="M23" s="417"/>
       <c r="O23" s="24" t="s">
         <v>68</v>
       </c>
@@ -10642,17 +10642,17 @@
       <c r="C51" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="382" t="s">
+      <c r="D51" s="416" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="382"/>
-      <c r="F51" s="382"/>
-      <c r="G51" s="382"/>
-      <c r="H51" s="382"/>
-      <c r="I51" s="382"/>
-      <c r="J51" s="382"/>
-      <c r="K51" s="382"/>
-      <c r="L51" s="383"/>
+      <c r="E51" s="416"/>
+      <c r="F51" s="416"/>
+      <c r="G51" s="416"/>
+      <c r="H51" s="416"/>
+      <c r="I51" s="416"/>
+      <c r="J51" s="416"/>
+      <c r="K51" s="416"/>
+      <c r="L51" s="417"/>
       <c r="M51"/>
       <c r="N51"/>
       <c r="O51"/>
@@ -32314,16 +32314,16 @@
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H136" s="385"/>
-      <c r="I136" s="384"/>
+      <c r="H136" s="382"/>
+      <c r="I136" s="381"/>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H137" s="385"/>
-      <c r="I137" s="384"/>
+      <c r="H137" s="382"/>
+      <c r="I137" s="381"/>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H138" s="385"/>
-      <c r="I138" s="384"/>
+      <c r="H138" s="382"/>
+      <c r="I138" s="381"/>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C139" s="155" t="s">
@@ -32352,7 +32352,7 @@
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C144" s="386" t="s">
+      <c r="C144" s="383" t="s">
         <v>140</v>
       </c>
       <c r="D144" s="85" t="s">
@@ -32533,43 +32533,43 @@
       </c>
       <c r="E171" s="115"/>
       <c r="F171" s="136">
-        <f>SUM(F163,F147,F130)</f>
+        <f t="shared" ref="F171:O171" si="114">SUM(F163,F147,F130)</f>
         <v>20</v>
       </c>
       <c r="G171" s="136">
-        <f>SUM(G163,G147,G130)</f>
+        <f t="shared" si="114"/>
         <v>80</v>
       </c>
       <c r="H171" s="136">
-        <f>SUM(H163,H147,H130)</f>
+        <f t="shared" si="114"/>
         <v>240</v>
       </c>
       <c r="I171" s="136">
-        <f>SUM(I163,I147,I130)</f>
+        <f t="shared" si="114"/>
         <v>170</v>
       </c>
       <c r="J171" s="136">
-        <f>SUM(J163,J147,J130)</f>
+        <f t="shared" si="114"/>
         <v>110</v>
       </c>
       <c r="K171" s="136">
-        <f>SUM(K163,K147,K130)</f>
+        <f t="shared" si="114"/>
         <v>60</v>
       </c>
       <c r="L171" s="136">
-        <f>SUM(L163,L147,L130)</f>
+        <f t="shared" si="114"/>
         <v>90</v>
       </c>
       <c r="M171" s="136">
-        <f>SUM(M163,M147,M130)</f>
+        <f t="shared" si="114"/>
         <v>70</v>
       </c>
       <c r="N171" s="136">
-        <f>SUM(N163,N147,N130)</f>
+        <f t="shared" si="114"/>
         <v>50</v>
       </c>
       <c r="O171" s="137">
-        <f>SUM(O163,O147,O130)</f>
+        <f t="shared" si="114"/>
         <v>20</v>
       </c>
       <c r="P171" t="s">
@@ -32600,43 +32600,43 @@
         <v>50</v>
       </c>
       <c r="F173" s="97">
-        <f t="shared" ref="F173:O173" si="114">E173+F172+F175-F171</f>
+        <f t="shared" ref="F173:O173" si="115">E173+F172+F175-F171</f>
         <v>30</v>
       </c>
       <c r="G173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>50</v>
       </c>
       <c r="H173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>60</v>
       </c>
       <c r="I173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>40</v>
       </c>
       <c r="J173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>30</v>
       </c>
       <c r="K173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>70</v>
       </c>
       <c r="L173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>30</v>
       </c>
       <c r="M173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>60</v>
       </c>
       <c r="N173" s="97">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>60</v>
       </c>
       <c r="O173" s="100">
-        <f t="shared" si="114"/>
+        <f t="shared" si="115"/>
         <v>40</v>
       </c>
     </row>
@@ -32646,43 +32646,43 @@
       </c>
       <c r="E174" s="116"/>
       <c r="F174" s="97">
-        <f t="shared" ref="F174:O174" si="115">IF(E173-F171&lt;=$E$127, F171-E173+$E$127,0)</f>
+        <f t="shared" ref="F174:O174" si="116">IF(E173-F171&lt;=$E$127, F171-E173+$E$127,0)</f>
         <v>0</v>
       </c>
       <c r="G174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>80</v>
       </c>
       <c r="H174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>220</v>
       </c>
       <c r="I174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>140</v>
       </c>
       <c r="J174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>100</v>
       </c>
       <c r="K174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>60</v>
       </c>
       <c r="L174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>50</v>
       </c>
       <c r="M174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>70</v>
       </c>
       <c r="N174" s="97">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>20</v>
       </c>
       <c r="O174" s="100">
-        <f t="shared" si="115"/>
+        <f t="shared" si="116"/>
         <v>0</v>
       </c>
     </row>
@@ -32692,43 +32692,43 @@
       </c>
       <c r="E175" s="116"/>
       <c r="F175" s="97">
-        <f t="shared" ref="F175:O175" si="116" xml:space="preserve"> CEILING(F174/$E$126,1)*$E$126</f>
+        <f t="shared" ref="F175:O175" si="117" xml:space="preserve"> CEILING(F174/$E$126,1)*$E$126</f>
         <v>0</v>
       </c>
       <c r="G175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>100</v>
       </c>
       <c r="H175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>250</v>
       </c>
       <c r="I175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>150</v>
       </c>
       <c r="J175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>100</v>
       </c>
       <c r="K175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>100</v>
       </c>
       <c r="L175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>50</v>
       </c>
       <c r="M175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>100</v>
       </c>
       <c r="N175" s="97">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>50</v>
       </c>
       <c r="O175" s="100">
-        <f t="shared" si="116"/>
+        <f t="shared" si="117"/>
         <v>0</v>
       </c>
     </row>
@@ -32746,35 +32746,35 @@
         <v>250</v>
       </c>
       <c r="H176" s="54">
-        <f t="shared" ref="H176:O176" si="117">I175</f>
+        <f t="shared" ref="H176:O176" si="118">I175</f>
         <v>150</v>
       </c>
       <c r="I176" s="54">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>100</v>
       </c>
       <c r="J176" s="54">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>100</v>
       </c>
       <c r="K176" s="54">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>50</v>
       </c>
       <c r="L176" s="54">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>100</v>
       </c>
       <c r="M176" s="54">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>50</v>
       </c>
       <c r="N176" s="54">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
       <c r="O176" s="55">
-        <f t="shared" si="117"/>
+        <f t="shared" si="118"/>
         <v>0</v>
       </c>
     </row>
@@ -32784,43 +32784,43 @@
       </c>
       <c r="E177" s="68"/>
       <c r="F177" s="65">
-        <f t="shared" ref="F177:O177" si="118">F171*$F$84</f>
+        <f t="shared" ref="F177:O177" si="119">F171*$F$84</f>
         <v>4000</v>
       </c>
       <c r="G177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>16000</v>
       </c>
       <c r="H177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>48000</v>
       </c>
       <c r="I177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>34000</v>
       </c>
       <c r="J177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>22000</v>
       </c>
       <c r="K177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>12000</v>
       </c>
       <c r="L177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>18000</v>
       </c>
       <c r="M177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>14000</v>
       </c>
       <c r="N177" s="65">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>10000</v>
       </c>
       <c r="O177" s="66">
-        <f t="shared" si="118"/>
+        <f t="shared" si="119"/>
         <v>4000</v>
       </c>
     </row>
@@ -32835,8 +32835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
   <dimension ref="A2:AI147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P63" sqref="P63"/>
+    <sheetView tabSelected="1" topLeftCell="D118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32979,7 +32979,7 @@
       <c r="O10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="409" t="s">
+      <c r="P10" s="406" t="s">
         <v>226</v>
       </c>
     </row>
@@ -32988,22 +32988,22 @@
         <v>162</v>
       </c>
       <c r="E11" s="276"/>
-      <c r="F11" s="396"/>
-      <c r="G11" s="396"/>
-      <c r="H11" s="396"/>
-      <c r="I11" s="396">
+      <c r="F11" s="393"/>
+      <c r="G11" s="393"/>
+      <c r="H11" s="393"/>
+      <c r="I11" s="393">
         <v>30</v>
       </c>
-      <c r="J11" s="411">
+      <c r="J11" s="408">
         <v>40</v>
       </c>
-      <c r="K11" s="396">
+      <c r="K11" s="393">
         <v>15</v>
       </c>
-      <c r="L11" s="396"/>
-      <c r="M11" s="396"/>
-      <c r="N11" s="396"/>
-      <c r="O11" s="397">
+      <c r="L11" s="393"/>
+      <c r="M11" s="393"/>
+      <c r="N11" s="393"/>
+      <c r="O11" s="394">
         <v>10</v>
       </c>
       <c r="P11" s="191" t="s">
@@ -33018,46 +33018,46 @@
         <v>204</v>
       </c>
       <c r="E12" s="278"/>
-      <c r="F12" s="398">
+      <c r="F12" s="395">
         <v>40</v>
       </c>
-      <c r="G12" s="398">
+      <c r="G12" s="395">
         <v>30</v>
       </c>
-      <c r="H12" s="398"/>
-      <c r="I12" s="398"/>
-      <c r="J12" s="398"/>
-      <c r="K12" s="398"/>
-      <c r="L12" s="398"/>
-      <c r="M12" s="398"/>
-      <c r="N12" s="398"/>
-      <c r="O12" s="399"/>
+      <c r="H12" s="395"/>
+      <c r="I12" s="395"/>
+      <c r="J12" s="395"/>
+      <c r="K12" s="395"/>
+      <c r="L12" s="395"/>
+      <c r="M12" s="395"/>
+      <c r="N12" s="395"/>
+      <c r="O12" s="396"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D13" s="279" t="s">
         <v>165</v>
       </c>
       <c r="E13" s="280"/>
-      <c r="F13" s="398"/>
-      <c r="G13" s="398"/>
-      <c r="H13" s="398">
-        <v>20</v>
-      </c>
-      <c r="I13" s="398">
+      <c r="F13" s="395"/>
+      <c r="G13" s="395"/>
+      <c r="H13" s="395">
+        <v>20</v>
+      </c>
+      <c r="I13" s="395">
         <v>50</v>
       </c>
-      <c r="J13" s="398">
+      <c r="J13" s="395">
         <v>60</v>
       </c>
-      <c r="K13" s="398"/>
-      <c r="L13" s="398">
+      <c r="K13" s="395"/>
+      <c r="L13" s="395">
         <v>40</v>
       </c>
-      <c r="M13" s="398"/>
-      <c r="N13" s="398">
+      <c r="M13" s="395"/>
+      <c r="N13" s="395">
         <v>40</v>
       </c>
-      <c r="O13" s="399"/>
+      <c r="O13" s="396"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14" s="251" t="s">
@@ -33067,20 +33067,20 @@
         <v>205</v>
       </c>
       <c r="E14" s="284"/>
-      <c r="F14" s="398">
+      <c r="F14" s="395">
         <v>50</v>
       </c>
-      <c r="G14" s="398">
+      <c r="G14" s="395">
         <v>40</v>
       </c>
-      <c r="H14" s="398"/>
-      <c r="I14" s="398"/>
-      <c r="J14" s="398"/>
-      <c r="K14" s="398"/>
-      <c r="L14" s="398"/>
-      <c r="M14" s="398"/>
-      <c r="N14" s="398"/>
-      <c r="O14" s="399"/>
+      <c r="H14" s="395"/>
+      <c r="I14" s="395"/>
+      <c r="J14" s="395"/>
+      <c r="K14" s="395"/>
+      <c r="L14" s="395"/>
+      <c r="M14" s="395"/>
+      <c r="N14" s="395"/>
+      <c r="O14" s="396"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="287" t="s">
@@ -33133,10 +33133,10 @@
         <v>203</v>
       </c>
       <c r="E16" s="263"/>
-      <c r="F16" s="402">
+      <c r="F16" s="399">
         <v>80</v>
       </c>
-      <c r="G16" s="402">
+      <c r="G16" s="399">
         <v>80</v>
       </c>
       <c r="H16" s="264"/>
@@ -33155,15 +33155,15 @@
       <c r="D17" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="E17" s="403">
+      <c r="E17" s="400">
         <v>50</v>
       </c>
       <c r="F17" s="267">
-        <f t="shared" ref="F17:O17" si="1">E17+F16+F19-F15</f>
+        <f>E17+F16+F19-F15</f>
         <v>40</v>
       </c>
       <c r="G17" s="267">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G17:O17" si="1">F17+G16+G19-G15</f>
         <v>50</v>
       </c>
       <c r="H17" s="267">
@@ -33484,34 +33484,34 @@
         <v>170</v>
       </c>
       <c r="E24" s="233"/>
-      <c r="F24" s="400">
+      <c r="F24" s="397">
         <v>210</v>
       </c>
-      <c r="G24" s="400">
+      <c r="G24" s="397">
         <v>211</v>
       </c>
-      <c r="H24" s="400">
+      <c r="H24" s="397">
         <v>213</v>
       </c>
-      <c r="I24" s="400">
+      <c r="I24" s="397">
         <v>215</v>
       </c>
-      <c r="J24" s="400">
+      <c r="J24" s="397">
         <v>215</v>
       </c>
-      <c r="K24" s="400">
+      <c r="K24" s="397">
         <v>216</v>
       </c>
-      <c r="L24" s="400">
+      <c r="L24" s="397">
         <v>214</v>
       </c>
-      <c r="M24" s="400">
+      <c r="M24" s="397">
         <v>212</v>
       </c>
-      <c r="N24" s="400">
+      <c r="N24" s="397">
         <v>210</v>
       </c>
-      <c r="O24" s="401">
+      <c r="O24" s="398">
         <v>209</v>
       </c>
     </row>
@@ -33627,34 +33627,34 @@
         <v>173</v>
       </c>
       <c r="E27" s="273"/>
-      <c r="F27" s="400">
+      <c r="F27" s="397">
         <v>410</v>
       </c>
-      <c r="G27" s="400">
+      <c r="G27" s="397">
         <v>413</v>
       </c>
-      <c r="H27" s="400">
+      <c r="H27" s="397">
         <v>410</v>
       </c>
-      <c r="I27" s="400">
+      <c r="I27" s="397">
         <v>415</v>
       </c>
-      <c r="J27" s="400">
+      <c r="J27" s="397">
         <v>418</v>
       </c>
-      <c r="K27" s="400">
+      <c r="K27" s="397">
         <v>430</v>
       </c>
-      <c r="L27" s="400">
+      <c r="L27" s="397">
         <v>423</v>
       </c>
-      <c r="M27" s="400">
+      <c r="M27" s="397">
         <v>419</v>
       </c>
-      <c r="N27" s="400">
+      <c r="N27" s="397">
         <v>417</v>
       </c>
-      <c r="O27" s="401">
+      <c r="O27" s="398">
         <v>422</v>
       </c>
     </row>
@@ -33862,7 +33862,7 @@
       </c>
       <c r="P31" s="251"/>
       <c r="AC31" s="6"/>
-      <c r="AD31" s="416"/>
+      <c r="AD31" s="413"/>
       <c r="AF31" s="349"/>
       <c r="AH31" s="349"/>
     </row>
@@ -35393,24 +35393,24 @@
         <v>162</v>
       </c>
       <c r="E51" s="276"/>
-      <c r="F51" s="395"/>
-      <c r="G51" s="395"/>
-      <c r="H51" s="395"/>
-      <c r="I51" s="410">
-        <v>20</v>
-      </c>
-      <c r="J51" s="395">
-        <v>20</v>
-      </c>
-      <c r="K51" s="395">
+      <c r="F51" s="392"/>
+      <c r="G51" s="392"/>
+      <c r="H51" s="392"/>
+      <c r="I51" s="407">
+        <v>20</v>
+      </c>
+      <c r="J51" s="392">
+        <v>20</v>
+      </c>
+      <c r="K51" s="392">
         <v>15</v>
       </c>
-      <c r="L51" s="395"/>
-      <c r="M51" s="395">
+      <c r="L51" s="392"/>
+      <c r="M51" s="392">
         <v>10</v>
       </c>
-      <c r="N51" s="395"/>
-      <c r="O51" s="395">
+      <c r="N51" s="392"/>
+      <c r="O51" s="392">
         <v>10</v>
       </c>
       <c r="S51" s="138"/>
@@ -35468,18 +35468,18 @@
         <v>204</v>
       </c>
       <c r="E52" s="278"/>
-      <c r="F52" s="395"/>
-      <c r="G52" s="395">
+      <c r="F52" s="392"/>
+      <c r="G52" s="392">
         <v>10</v>
       </c>
-      <c r="H52" s="395"/>
-      <c r="I52" s="395"/>
-      <c r="J52" s="395"/>
-      <c r="K52" s="395"/>
-      <c r="L52" s="395"/>
-      <c r="M52" s="395"/>
-      <c r="N52" s="395"/>
-      <c r="O52" s="395"/>
+      <c r="H52" s="392"/>
+      <c r="I52" s="392"/>
+      <c r="J52" s="392"/>
+      <c r="K52" s="392"/>
+      <c r="L52" s="392"/>
+      <c r="M52" s="392"/>
+      <c r="N52" s="392"/>
+      <c r="O52" s="392"/>
       <c r="S52" s="138"/>
       <c r="T52" s="138"/>
       <c r="V52" s="138">
@@ -35535,24 +35535,24 @@
         <v>165</v>
       </c>
       <c r="E53" s="280"/>
-      <c r="F53" s="395"/>
-      <c r="G53" s="395"/>
-      <c r="H53" s="395"/>
-      <c r="I53" s="395">
+      <c r="F53" s="392"/>
+      <c r="G53" s="392"/>
+      <c r="H53" s="392"/>
+      <c r="I53" s="392">
         <v>60</v>
       </c>
-      <c r="J53" s="395">
+      <c r="J53" s="392">
         <v>80</v>
       </c>
-      <c r="K53" s="395"/>
-      <c r="L53" s="395">
+      <c r="K53" s="392"/>
+      <c r="L53" s="392">
         <v>40</v>
       </c>
-      <c r="M53" s="395"/>
-      <c r="N53" s="395">
+      <c r="M53" s="392"/>
+      <c r="N53" s="392">
         <v>50</v>
       </c>
-      <c r="O53" s="395"/>
+      <c r="O53" s="392"/>
       <c r="S53" s="138"/>
       <c r="T53" s="138"/>
       <c r="V53" s="138">
@@ -35608,18 +35608,18 @@
         <v>205</v>
       </c>
       <c r="E54" s="284"/>
-      <c r="F54" s="395"/>
-      <c r="G54" s="395">
+      <c r="F54" s="392"/>
+      <c r="G54" s="392">
         <v>40</v>
       </c>
-      <c r="H54" s="395"/>
-      <c r="I54" s="395"/>
-      <c r="J54" s="395"/>
-      <c r="K54" s="395"/>
-      <c r="L54" s="395"/>
-      <c r="M54" s="395"/>
-      <c r="N54" s="395"/>
-      <c r="O54" s="395"/>
+      <c r="H54" s="392"/>
+      <c r="I54" s="392"/>
+      <c r="J54" s="392"/>
+      <c r="K54" s="392"/>
+      <c r="L54" s="392"/>
+      <c r="M54" s="392"/>
+      <c r="N54" s="392"/>
+      <c r="O54" s="392"/>
       <c r="S54" s="138"/>
       <c r="T54" s="138"/>
       <c r="V54" s="138">
@@ -35770,10 +35770,10 @@
         <v>203</v>
       </c>
       <c r="E56" s="263"/>
-      <c r="F56" s="402">
-        <v>20</v>
-      </c>
-      <c r="G56" s="402"/>
+      <c r="F56" s="399">
+        <v>20</v>
+      </c>
+      <c r="G56" s="399"/>
       <c r="H56" s="264"/>
       <c r="I56" s="264"/>
       <c r="J56" s="264"/>
@@ -35834,7 +35834,7 @@
       <c r="D57" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="E57" s="403">
+      <c r="E57" s="400">
         <v>30</v>
       </c>
       <c r="F57" s="267">
@@ -36478,38 +36478,38 @@
       </c>
     </row>
     <row r="64" spans="3:34" x14ac:dyDescent="0.3">
-      <c r="D64" s="404" t="s">
+      <c r="D64" s="401" t="s">
         <v>170</v>
       </c>
       <c r="E64" s="233"/>
-      <c r="F64" s="407">
+      <c r="F64" s="404">
         <v>210</v>
       </c>
-      <c r="G64" s="407">
+      <c r="G64" s="404">
         <v>211</v>
       </c>
-      <c r="H64" s="407">
+      <c r="H64" s="404">
         <v>213</v>
       </c>
-      <c r="I64" s="407">
+      <c r="I64" s="404">
         <v>215</v>
       </c>
-      <c r="J64" s="407">
+      <c r="J64" s="404">
         <v>215</v>
       </c>
-      <c r="K64" s="407">
+      <c r="K64" s="404">
         <v>216</v>
       </c>
-      <c r="L64" s="407">
+      <c r="L64" s="404">
         <v>214</v>
       </c>
-      <c r="M64" s="407">
+      <c r="M64" s="404">
         <v>212</v>
       </c>
-      <c r="N64" s="407">
+      <c r="N64" s="404">
         <v>210</v>
       </c>
-      <c r="O64" s="408">
+      <c r="O64" s="405">
         <v>209</v>
       </c>
       <c r="W64" s="138">
@@ -36560,7 +36560,7 @@
       <c r="C65" s="251" t="s">
         <v>181</v>
       </c>
-      <c r="D65" s="405" t="s">
+      <c r="D65" s="402" t="s">
         <v>171</v>
       </c>
       <c r="E65" s="243"/>
@@ -36652,7 +36652,7 @@
       </c>
     </row>
     <row r="66" spans="3:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D66" s="406" t="s">
+      <c r="D66" s="403" t="s">
         <v>172</v>
       </c>
       <c r="E66" s="255"/>
@@ -36748,34 +36748,34 @@
         <v>173</v>
       </c>
       <c r="E67" s="273"/>
-      <c r="F67" s="400">
+      <c r="F67" s="397">
         <v>411</v>
       </c>
-      <c r="G67" s="400">
+      <c r="G67" s="397">
         <v>414</v>
       </c>
-      <c r="H67" s="400">
+      <c r="H67" s="397">
         <v>412</v>
       </c>
-      <c r="I67" s="400">
+      <c r="I67" s="397">
         <v>413</v>
       </c>
-      <c r="J67" s="400">
+      <c r="J67" s="397">
         <v>418</v>
       </c>
-      <c r="K67" s="400">
+      <c r="K67" s="397">
         <v>428</v>
       </c>
-      <c r="L67" s="400">
+      <c r="L67" s="397">
         <v>426</v>
       </c>
-      <c r="M67" s="400">
+      <c r="M67" s="397">
         <v>419</v>
       </c>
-      <c r="N67" s="400">
+      <c r="N67" s="397">
         <v>415</v>
       </c>
-      <c r="O67" s="401">
+      <c r="O67" s="398">
         <v>421</v>
       </c>
       <c r="W67" s="138">
@@ -37007,47 +37007,47 @@
       </c>
     </row>
     <row r="70" spans="3:35" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D70" s="412" t="s">
+      <c r="D70" s="409" t="s">
         <v>193</v>
       </c>
-      <c r="E70" s="413"/>
-      <c r="F70" s="414">
+      <c r="E70" s="410"/>
+      <c r="F70" s="411">
         <f>SUM(G51:G52)</f>
         <v>10</v>
       </c>
-      <c r="G70" s="414">
+      <c r="G70" s="411">
         <f t="shared" ref="G70:O70" si="46">SUM(H51:H52)</f>
         <v>0</v>
       </c>
-      <c r="H70" s="414">
+      <c r="H70" s="411">
         <f t="shared" si="46"/>
         <v>20</v>
       </c>
-      <c r="I70" s="414">
+      <c r="I70" s="411">
         <f t="shared" si="46"/>
         <v>20</v>
       </c>
-      <c r="J70" s="414">
+      <c r="J70" s="411">
         <f t="shared" si="46"/>
         <v>15</v>
       </c>
-      <c r="K70" s="414">
+      <c r="K70" s="411">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="L70" s="414">
+      <c r="L70" s="411">
         <f t="shared" si="46"/>
         <v>10</v>
       </c>
-      <c r="M70" s="414">
+      <c r="M70" s="411">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="N70" s="414">
+      <c r="N70" s="411">
         <f t="shared" si="46"/>
         <v>10</v>
       </c>
-      <c r="O70" s="415">
+      <c r="O70" s="412">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -37754,43 +37754,43 @@
       </c>
       <c r="E80" s="329"/>
       <c r="F80" s="330">
-        <f>F70/F60</f>
+        <f t="shared" ref="F80:O80" si="56">F70/F60</f>
         <v>0.5</v>
       </c>
       <c r="G80" s="330" t="e">
-        <f>G70/G60</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H80" s="330">
-        <f>H70/H60</f>
+        <f t="shared" si="56"/>
         <v>0.25</v>
       </c>
       <c r="I80" s="330">
-        <f>I70/I60</f>
+        <f t="shared" si="56"/>
         <v>0.2</v>
       </c>
       <c r="J80" s="330">
-        <f>J70/J60</f>
+        <f t="shared" si="56"/>
         <v>0.75</v>
       </c>
       <c r="K80" s="330">
-        <f>K70/K60</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="L80" s="330">
-        <f>L70/L60</f>
+        <f t="shared" si="56"/>
         <v>0.5</v>
       </c>
       <c r="M80" s="330">
-        <f>M70/M60</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="N80" s="330">
-        <f>N70/N60</f>
+        <f t="shared" si="56"/>
         <v>0.5</v>
       </c>
       <c r="O80" s="330" t="e">
-        <f>O70/O60</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA80" s="367"/>
@@ -37801,43 +37801,43 @@
       </c>
       <c r="E81" s="329"/>
       <c r="F81" s="330">
-        <f>F76/F66</f>
+        <f t="shared" ref="F81:O81" si="57">F76/F66</f>
         <v>0</v>
       </c>
       <c r="G81" s="330" t="e">
-        <f>G76/G66</f>
+        <f t="shared" si="57"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H81" s="330">
-        <f>H76/H66</f>
+        <f t="shared" si="57"/>
         <v>0.25</v>
       </c>
       <c r="I81" s="330">
-        <f>I76/I66</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="J81" s="330">
-        <f>J76/J66</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="K81" s="330">
-        <f>K76/K66</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="L81" s="330">
-        <f>L76/L66</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="M81" s="330">
-        <f>M76/M66</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="N81" s="330">
-        <f>N76/N66</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="O81" s="330" t="e">
-        <f>O76/O66</f>
+        <f t="shared" si="57"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W81"/>
@@ -37858,43 +37858,43 @@
       </c>
       <c r="E82" s="331"/>
       <c r="F82" s="332">
-        <f>F78/F69</f>
+        <f t="shared" ref="F82:O82" si="58">F78/F69</f>
         <v>0</v>
       </c>
       <c r="G82" s="332" t="e">
-        <f>G78/G69</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H82" s="332">
-        <f>H78/H69</f>
+        <f t="shared" si="58"/>
         <v>0.25</v>
       </c>
       <c r="I82" s="332">
-        <f>I78/I69</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="J82" s="332">
-        <f>J78/J69</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="K82" s="332">
-        <f>K78/K69</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="L82" s="332">
-        <f>L78/L69</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="M82" s="332">
-        <f>M78/M69</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="N82" s="332">
-        <f>N78/N69</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="O82" s="332" t="e">
-        <f>O78/O69</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W82" s="138"/>
@@ -38172,39 +38172,39 @@
         <v>10</v>
       </c>
       <c r="G96" s="289">
-        <f t="shared" ref="G96:O96" si="56">SUM(G92:G95)</f>
+        <f t="shared" ref="G96:O96" si="59">SUM(G92:G95)</f>
         <v>20</v>
       </c>
       <c r="H96" s="289">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>55</v>
       </c>
       <c r="I96" s="289">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>50</v>
       </c>
       <c r="J96" s="289">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>50</v>
       </c>
       <c r="K96" s="289">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>20</v>
       </c>
       <c r="L96" s="289">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>30</v>
       </c>
       <c r="M96" s="289">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>15</v>
       </c>
       <c r="N96" s="289">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>30</v>
       </c>
       <c r="O96" s="290">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>20</v>
       </c>
     </row>
@@ -38238,39 +38238,39 @@
         <v>30</v>
       </c>
       <c r="G98" s="97">
-        <f t="shared" ref="G98:O98" si="57">F98+G97+G100-G96</f>
+        <f t="shared" ref="G98:O98" si="60">F98+G97+G100-G96</f>
         <v>10</v>
       </c>
       <c r="H98" s="97">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>15</v>
       </c>
       <c r="I98" s="97">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>15</v>
       </c>
       <c r="J98" s="97">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>15</v>
       </c>
       <c r="K98" s="97">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>15</v>
       </c>
       <c r="L98" s="97">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>15</v>
       </c>
       <c r="M98" s="97">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>10</v>
       </c>
       <c r="N98" s="97">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>10</v>
       </c>
       <c r="O98" s="100">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>10</v>
       </c>
       <c r="Q98" s="341" t="s">
@@ -38287,39 +38287,39 @@
         <v>0</v>
       </c>
       <c r="G99" s="97">
-        <f t="shared" ref="G99:O99" si="58">IF(F98-G96&lt;=$E$90, G96-F98+$E$90,0)</f>
+        <f t="shared" ref="G99:O99" si="61">IF(F98-G96&lt;=$E$90, G96-F98+$E$90,0)</f>
         <v>0</v>
       </c>
       <c r="H99" s="97">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>55</v>
       </c>
       <c r="I99" s="97">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>45</v>
       </c>
       <c r="J99" s="97">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>45</v>
       </c>
       <c r="K99" s="97">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>15</v>
       </c>
       <c r="L99" s="97">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>25</v>
       </c>
       <c r="M99" s="97">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>10</v>
       </c>
       <c r="N99" s="97">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>30</v>
       </c>
       <c r="O99" s="100">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>20</v>
       </c>
       <c r="Q99" s="342" t="s">
@@ -38336,39 +38336,39 @@
         <v>0</v>
       </c>
       <c r="G100" s="97">
-        <f t="shared" ref="G100:O100" si="59" xml:space="preserve"> CEILING(G99/$E$89,1)*$E$89</f>
+        <f t="shared" ref="G100:O100" si="62" xml:space="preserve"> CEILING(G99/$E$89,1)*$E$89</f>
         <v>0</v>
       </c>
       <c r="H100" s="97">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>60</v>
       </c>
       <c r="I100" s="97">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>50</v>
       </c>
       <c r="J100" s="97">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>50</v>
       </c>
       <c r="K100" s="97">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>20</v>
       </c>
       <c r="L100" s="97">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>30</v>
       </c>
       <c r="M100" s="97">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>10</v>
       </c>
       <c r="N100" s="97">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>30</v>
       </c>
       <c r="O100" s="100">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>20</v>
       </c>
     </row>
@@ -38378,43 +38378,43 @@
       </c>
       <c r="E101" s="380"/>
       <c r="F101" s="271">
-        <f t="shared" ref="F101:O101" si="60">F100</f>
+        <f t="shared" ref="F101:O101" si="63">F100</f>
         <v>0</v>
       </c>
       <c r="G101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="H101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>60</v>
       </c>
       <c r="I101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>50</v>
       </c>
       <c r="J101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>50</v>
       </c>
       <c r="K101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>20</v>
       </c>
       <c r="L101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>30</v>
       </c>
       <c r="M101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>10</v>
       </c>
       <c r="N101" s="271">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>30</v>
       </c>
       <c r="O101" s="272">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>20</v>
       </c>
     </row>
@@ -38428,39 +38428,39 @@
         <v>0</v>
       </c>
       <c r="G102" s="370">
-        <f t="shared" ref="G102:O102" si="61">QUOTIENT(MOD(G101+$E$87-1,$E$86),$E$87)</f>
+        <f t="shared" ref="G102:O102" si="64">QUOTIENT(MOD(G101+$E$87-1,$E$86),$E$87)</f>
         <v>0</v>
       </c>
       <c r="H102" s="370">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I102" s="370">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="J102" s="370">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="K102" s="370">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="L102" s="370">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="M102" s="370">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="N102" s="370">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="O102" s="371">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
     </row>
@@ -38475,39 +38475,39 @@
         <v>0</v>
       </c>
       <c r="G103" s="313">
-        <f t="shared" ref="G103:O103" si="62">QUOTIENT(G101+$E$87-1,$E$86)</f>
+        <f t="shared" ref="G103:O103" si="65">QUOTIENT(G101+$E$87-1,$E$86)</f>
         <v>0</v>
       </c>
       <c r="H103" s="313">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>3</v>
       </c>
       <c r="I103" s="313">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>2</v>
       </c>
       <c r="J103" s="313">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>2</v>
       </c>
       <c r="K103" s="313">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1</v>
       </c>
       <c r="L103" s="313">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1</v>
       </c>
       <c r="M103" s="313">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="N103" s="313">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1</v>
       </c>
       <c r="O103" s="314">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>1</v>
       </c>
     </row>
@@ -38521,39 +38521,39 @@
         <v>0</v>
       </c>
       <c r="G104" s="373">
-        <f t="shared" ref="G104:O104" si="63">G103*$F$86+G102*$F$87</f>
+        <f t="shared" ref="G104:O104" si="66">G103*$F$86+G102*$F$87</f>
         <v>0</v>
       </c>
       <c r="H104" s="373">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>600</v>
       </c>
       <c r="I104" s="373">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>520</v>
       </c>
       <c r="J104" s="373">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>520</v>
       </c>
       <c r="K104" s="373">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>200</v>
       </c>
       <c r="L104" s="373">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>320</v>
       </c>
       <c r="M104" s="373">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>120</v>
       </c>
       <c r="N104" s="373">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>320</v>
       </c>
       <c r="O104" s="374">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>200</v>
       </c>
     </row>
@@ -38606,39 +38606,39 @@
         <v>0</v>
       </c>
       <c r="G106" s="333">
-        <f t="shared" ref="G106:O106" si="64">G105*G101</f>
+        <f t="shared" ref="G106:O106" si="67">G105*G101</f>
         <v>0</v>
       </c>
       <c r="H106" s="333">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>12780</v>
       </c>
       <c r="I106" s="333">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>10750</v>
       </c>
       <c r="J106" s="333">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>10750</v>
       </c>
       <c r="K106" s="333">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>4320</v>
       </c>
       <c r="L106" s="333">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>6420</v>
       </c>
       <c r="M106" s="333">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>2120</v>
       </c>
       <c r="N106" s="333">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>6300</v>
       </c>
       <c r="O106" s="377">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>4180</v>
       </c>
       <c r="P106" s="251" t="s">
@@ -38651,43 +38651,43 @@
       </c>
       <c r="E107" s="255"/>
       <c r="F107" s="336">
-        <f t="shared" ref="F107:O107" si="65">F104+F106</f>
+        <f t="shared" ref="F107:O107" si="68">F104+F106</f>
         <v>0</v>
       </c>
       <c r="G107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="H107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>13380</v>
       </c>
       <c r="I107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>11270</v>
       </c>
       <c r="J107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>11270</v>
       </c>
       <c r="K107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>4520</v>
       </c>
       <c r="L107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>6740</v>
       </c>
       <c r="M107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>2240</v>
       </c>
       <c r="N107" s="336">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>6620</v>
       </c>
       <c r="O107" s="337">
-        <f t="shared" si="65"/>
+        <f t="shared" si="68"/>
         <v>4380</v>
       </c>
       <c r="P107" s="251" t="s">
@@ -38740,39 +38740,39 @@
         <v>0</v>
       </c>
       <c r="G109" s="338">
-        <f t="shared" ref="G109:O109" si="66">G108*G101</f>
+        <f t="shared" ref="G109:O109" si="69">G108*G101</f>
         <v>0</v>
       </c>
       <c r="H109" s="338">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>24600</v>
       </c>
       <c r="I109" s="338">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>20750</v>
       </c>
       <c r="J109" s="338">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>20900</v>
       </c>
       <c r="K109" s="338">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>8600</v>
       </c>
       <c r="L109" s="338">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>12690</v>
       </c>
       <c r="M109" s="338">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>4190</v>
       </c>
       <c r="N109" s="338">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>12510</v>
       </c>
       <c r="O109" s="339">
-        <f t="shared" si="66"/>
+        <f t="shared" si="69"/>
         <v>8440</v>
       </c>
       <c r="P109" s="251" t="s">
@@ -38789,39 +38789,39 @@
         <v>0</v>
       </c>
       <c r="G110" s="292">
-        <f t="shared" ref="G110:O110" si="67">G109-G107</f>
+        <f t="shared" ref="G110:O110" si="70">G109-G107</f>
         <v>0</v>
       </c>
       <c r="H110" s="292">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>11220</v>
       </c>
       <c r="I110" s="292">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>9480</v>
       </c>
       <c r="J110" s="292">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>9630</v>
       </c>
       <c r="K110" s="292">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>4080</v>
       </c>
       <c r="L110" s="292">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>5950</v>
       </c>
       <c r="M110" s="292">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>1950</v>
       </c>
       <c r="N110" s="292">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>5890</v>
       </c>
       <c r="O110" s="293">
-        <f t="shared" si="67"/>
+        <f t="shared" si="70"/>
         <v>4060</v>
       </c>
       <c r="P110" s="251" t="s">
@@ -38829,48 +38829,48 @@
       </c>
     </row>
     <row r="111" spans="3:35" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D111" s="412" t="s">
+      <c r="D111" s="409" t="s">
         <v>193</v>
       </c>
-      <c r="E111" s="413"/>
-      <c r="F111" s="414">
+      <c r="E111" s="410"/>
+      <c r="F111" s="411">
         <f>SUM(F92:F93)</f>
         <v>10</v>
       </c>
-      <c r="G111" s="414">
-        <f t="shared" ref="G111:O111" si="68">SUM(G92:G93)</f>
-        <v>0</v>
-      </c>
-      <c r="H111" s="414">
-        <f t="shared" si="68"/>
+      <c r="G111" s="411">
+        <f t="shared" ref="G111:O111" si="71">SUM(G92:G93)</f>
+        <v>0</v>
+      </c>
+      <c r="H111" s="411">
+        <f t="shared" si="71"/>
         <v>15</v>
       </c>
-      <c r="I111" s="414">
-        <f t="shared" si="68"/>
-        <v>20</v>
-      </c>
-      <c r="J111" s="414">
-        <f t="shared" si="68"/>
+      <c r="I111" s="411">
+        <f t="shared" si="71"/>
+        <v>20</v>
+      </c>
+      <c r="J111" s="411">
+        <f t="shared" si="71"/>
         <v>10</v>
       </c>
-      <c r="K111" s="414">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="L111" s="414">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="M111" s="414">
-        <f t="shared" si="68"/>
+      <c r="K111" s="411">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="L111" s="411">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="M111" s="411">
+        <f t="shared" si="71"/>
         <v>15</v>
       </c>
-      <c r="N111" s="414">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="O111" s="415">
-        <f t="shared" si="68"/>
+      <c r="N111" s="411">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="O111" s="412">
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="P111" s="251" t="s">
@@ -38896,11 +38896,11 @@
       </c>
       <c r="E112" s="307"/>
       <c r="F112" s="258">
-        <f t="shared" ref="F112:G112" si="69">MIN(F139,F111)</f>
+        <f t="shared" ref="F112:G112" si="72">MIN(F139,F111)</f>
         <v>0</v>
       </c>
       <c r="G112" s="258">
-        <f t="shared" si="69"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="H112" s="258">
@@ -38908,31 +38908,31 @@
         <v>15</v>
       </c>
       <c r="I112" s="258">
-        <f t="shared" ref="I112" si="70">MIN(I139,I111)</f>
+        <f t="shared" ref="I112" si="73">MIN(I139,I111)</f>
         <v>0</v>
       </c>
       <c r="J112" s="258">
-        <f t="shared" ref="J112:K112" si="71">MIN(J139,J111)</f>
+        <f t="shared" ref="J112:K112" si="74">MIN(J139,J111)</f>
         <v>0</v>
       </c>
       <c r="K112" s="258">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="L112" s="258">
-        <f t="shared" ref="L112" si="72">MIN(L139,L111)</f>
+        <f t="shared" ref="L112" si="75">MIN(L139,L111)</f>
         <v>0</v>
       </c>
       <c r="M112" s="258">
-        <f t="shared" ref="M112:N112" si="73">MIN(M139,M111)</f>
+        <f t="shared" ref="M112:N112" si="76">MIN(M139,M111)</f>
         <v>0</v>
       </c>
       <c r="N112" s="258">
-        <f t="shared" si="73"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="O112" s="259">
-        <f t="shared" ref="O112" si="74">MIN(O139,O111)</f>
+        <f t="shared" ref="O112" si="77">MIN(O139,O111)</f>
         <v>0</v>
       </c>
       <c r="P112" s="251" t="s">
@@ -38942,15 +38942,15 @@
         <v>38</v>
       </c>
       <c r="X112" s="138">
-        <f t="shared" ref="X112" si="75">CEILING(W112,20)</f>
+        <f t="shared" ref="X112" si="78">CEILING(W112,20)</f>
         <v>40</v>
       </c>
       <c r="Y112" s="138">
-        <f t="shared" ref="Y112" si="76">FLOOR(W112,20)</f>
+        <f t="shared" ref="Y112" si="79">FLOOR(W112,20)</f>
         <v>20</v>
       </c>
       <c r="Z112" s="138">
-        <f t="shared" ref="Z112" si="77">MOD(W112,20)</f>
+        <f t="shared" ref="Z112" si="80">MOD(W112,20)</f>
         <v>18</v>
       </c>
       <c r="AA112" s="3">
@@ -38966,19 +38966,19 @@
         <v>2</v>
       </c>
       <c r="AE112" s="357">
-        <f t="shared" ref="AE112" si="78">QUOTIENT(MOD(W112,$AD$26),$AD$25)</f>
+        <f t="shared" ref="AE112" si="81">QUOTIENT(MOD(W112,$AD$26),$AD$25)</f>
         <v>1</v>
       </c>
       <c r="AF112" s="358">
-        <f t="shared" ref="AF112" si="79">QUOTIENT(MOD(W112+$AD$25-1,$AD$26),$AD$25)</f>
+        <f t="shared" ref="AF112" si="82">QUOTIENT(MOD(W112+$AD$25-1,$AD$26),$AD$25)</f>
         <v>0</v>
       </c>
       <c r="AG112" s="357">
-        <f t="shared" ref="AG112" si="80">QUOTIENT(W112,$AD$26)</f>
+        <f t="shared" ref="AG112" si="83">QUOTIENT(W112,$AD$26)</f>
         <v>1</v>
       </c>
       <c r="AH112" s="359">
-        <f t="shared" ref="AH112" si="81">QUOTIENT(W112+$AD$25-1,$AD$26)</f>
+        <f t="shared" ref="AH112" si="84">QUOTIENT(W112+$AD$25-1,$AD$26)</f>
         <v>2</v>
       </c>
       <c r="AI112" s="138"/>
@@ -38993,39 +38993,39 @@
         <v>0</v>
       </c>
       <c r="G113" s="369">
-        <f t="shared" ref="G113:O113" si="82">QUOTIENT(MOD(G112+$E$87-1,$E$86),$E$87)</f>
+        <f t="shared" ref="G113:O113" si="85">QUOTIENT(MOD(G112+$E$87-1,$E$86),$E$87)</f>
         <v>0</v>
       </c>
       <c r="H113" s="369">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="I113" s="369">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="J113" s="369">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="K113" s="369">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="L113" s="369">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="M113" s="369">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="N113" s="369">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="O113" s="378">
-        <f t="shared" si="82"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="P113" s="191"/>
@@ -39040,39 +39040,39 @@
         <v>0</v>
       </c>
       <c r="G114" s="313">
-        <f t="shared" ref="G114:O114" si="83">QUOTIENT(G112+$E$87-1,$E$86)</f>
+        <f t="shared" ref="G114:O114" si="86">QUOTIENT(G112+$E$87-1,$E$86)</f>
         <v>0</v>
       </c>
       <c r="H114" s="313">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>1</v>
       </c>
       <c r="I114" s="313">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="J114" s="313">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="K114" s="313">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="L114" s="313">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="M114" s="313">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="N114" s="313">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="O114" s="314">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="P114" s="191"/>
@@ -39087,39 +39087,39 @@
         <v>0</v>
       </c>
       <c r="G115" s="316">
-        <f t="shared" ref="G115:O115" si="84">G114*$F$86+G113*$F$87</f>
+        <f t="shared" ref="G115:O115" si="87">G114*$F$86+G113*$F$87</f>
         <v>0</v>
       </c>
       <c r="H115" s="316">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>200</v>
       </c>
       <c r="I115" s="316">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="J115" s="316">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="K115" s="316">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="L115" s="316">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="M115" s="316">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="N115" s="316">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="O115" s="317">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="P115" s="177"/>
@@ -39137,39 +39137,39 @@
         <v>0</v>
       </c>
       <c r="G116" s="194">
-        <f t="shared" ref="G116:O116" si="85">G112*G105</f>
+        <f t="shared" ref="G116:O116" si="88">G112*G105</f>
         <v>0</v>
       </c>
       <c r="H116" s="194">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>3195</v>
       </c>
       <c r="I116" s="194">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="J116" s="194">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="K116" s="194">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="L116" s="194">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="M116" s="194">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="N116" s="194">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O116" s="195">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="P116" s="177"/>
@@ -39185,39 +39185,39 @@
         <v>0</v>
       </c>
       <c r="G117" s="292">
-        <f t="shared" ref="G117:O117" si="86">G116+G115</f>
+        <f t="shared" ref="G117:O117" si="89">G116+G115</f>
         <v>0</v>
       </c>
       <c r="H117" s="292">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>3395</v>
       </c>
       <c r="I117" s="292">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="J117" s="292">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="K117" s="292">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="L117" s="292">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="M117" s="292">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="N117" s="292">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="O117" s="293">
-        <f t="shared" si="86"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="P117" s="191"/>
@@ -39232,39 +39232,39 @@
         <v>0</v>
       </c>
       <c r="G118" s="194">
-        <f t="shared" ref="G118:O118" si="87">G112*G108</f>
+        <f t="shared" ref="G118:O118" si="90">G112*G108</f>
         <v>0</v>
       </c>
       <c r="H118" s="194">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>6150</v>
       </c>
       <c r="I118" s="194">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="J118" s="194">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="K118" s="194">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="L118" s="194">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="M118" s="194">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="N118" s="194">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="O118" s="195">
-        <f t="shared" si="87"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="P118" s="191"/>
@@ -39283,35 +39283,35 @@
         <v>0</v>
       </c>
       <c r="H119" s="340">
-        <f t="shared" ref="H119:O119" si="88">H118-H117</f>
+        <f t="shared" ref="H119:O119" si="91">H118-H117</f>
         <v>2755</v>
       </c>
       <c r="I119" s="326">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="J119" s="326">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="K119" s="326">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L119" s="326">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="M119" s="326">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="N119" s="326">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="O119" s="327">
-        <f t="shared" si="88"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="P119" s="251" t="s">
@@ -39332,35 +39332,35 @@
         <v>0</v>
       </c>
       <c r="H120" s="224">
-        <f t="shared" ref="H120:O120" si="89">H110-H119</f>
+        <f t="shared" ref="H120:O120" si="92">H110-H119</f>
         <v>8465</v>
       </c>
       <c r="I120" s="224">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>9480</v>
       </c>
       <c r="J120" s="224">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>9630</v>
       </c>
       <c r="K120" s="224">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>4080</v>
       </c>
       <c r="L120" s="224">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>5950</v>
       </c>
       <c r="M120" s="224">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>1950</v>
       </c>
       <c r="N120" s="224">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>5890</v>
       </c>
       <c r="O120" s="225">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>4060</v>
       </c>
       <c r="AA120" s="367"/>
@@ -39375,39 +39375,39 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G121" s="330" t="e">
-        <f t="shared" ref="G121:O121" si="90">G111/G101</f>
+        <f t="shared" ref="G121:O121" si="93">G111/G101</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>0.25</v>
       </c>
       <c r="I121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>0.4</v>
       </c>
       <c r="J121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>0.2</v>
       </c>
       <c r="K121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="L121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="M121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>1.5</v>
       </c>
       <c r="N121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="O121" s="330">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AA121" s="367"/>
@@ -39422,39 +39422,39 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G122" s="330" t="e">
-        <f t="shared" ref="G122:O122" si="91">G117/G107</f>
+        <f t="shared" ref="G122:O122" si="94">G117/G107</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.2537369207772795</v>
       </c>
       <c r="I122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="J122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="K122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="M122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="N122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O122" s="330">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="W122"/>
@@ -39479,7 +39479,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G123" s="332" t="e">
-        <f t="shared" ref="G123:O123" si="92">G119/G110</f>
+        <f t="shared" ref="G123:O123" si="95">G119/G110</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H123" s="332">
@@ -39487,31 +39487,31 @@
         <v>0.24554367201426025</v>
       </c>
       <c r="I123" s="332">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="J123" s="332">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="K123" s="332">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="L123" s="332">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="M123" s="332">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="N123" s="332">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="O123" s="332">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="W123" s="138"/>
@@ -39665,43 +39665,43 @@
       </c>
       <c r="E133" s="115"/>
       <c r="F133" s="136">
-        <f>SUM(F101,F60,F20)</f>
+        <f t="shared" ref="F133:O133" si="96">SUM(F101,F60,F20)</f>
         <v>20</v>
       </c>
       <c r="G133" s="136">
-        <f>SUM(G101,G60,G20)</f>
+        <f t="shared" si="96"/>
         <v>80</v>
       </c>
       <c r="H133" s="136">
-        <f>SUM(H101,H60,H20)</f>
+        <f t="shared" si="96"/>
         <v>240</v>
       </c>
       <c r="I133" s="136">
-        <f>SUM(I101,I60,I20)</f>
+        <f t="shared" si="96"/>
         <v>170</v>
       </c>
       <c r="J133" s="136">
-        <f>SUM(J101,J60,J20)</f>
+        <f t="shared" si="96"/>
         <v>110</v>
       </c>
       <c r="K133" s="136">
-        <f>SUM(K101,K60,K20)</f>
+        <f t="shared" si="96"/>
         <v>60</v>
       </c>
       <c r="L133" s="136">
-        <f>SUM(L101,L60,L20)</f>
+        <f t="shared" si="96"/>
         <v>90</v>
       </c>
       <c r="M133" s="136">
-        <f>SUM(M101,M60,M20)</f>
+        <f t="shared" si="96"/>
         <v>70</v>
       </c>
       <c r="N133" s="136">
-        <f>SUM(N101,N60,N20)</f>
+        <f t="shared" si="96"/>
         <v>50</v>
       </c>
       <c r="O133" s="137">
-        <f>SUM(O101,O60,O20)</f>
+        <f t="shared" si="96"/>
         <v>20</v>
       </c>
     </row>
@@ -39729,43 +39729,43 @@
         <v>50</v>
       </c>
       <c r="F135" s="267">
-        <f t="shared" ref="F135:O135" si="93">E135+F137-F133</f>
+        <f t="shared" ref="F135:O135" si="97">E135+F137-F133</f>
         <v>30</v>
       </c>
       <c r="G135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>50</v>
       </c>
       <c r="H135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>60</v>
       </c>
       <c r="I135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>40</v>
       </c>
       <c r="J135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>30</v>
       </c>
       <c r="K135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>70</v>
       </c>
       <c r="L135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>30</v>
       </c>
       <c r="M135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>60</v>
       </c>
       <c r="N135" s="267">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>60</v>
       </c>
       <c r="O135" s="268">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>40</v>
       </c>
     </row>
@@ -39775,43 +39775,43 @@
       </c>
       <c r="E136" s="266"/>
       <c r="F136" s="267">
-        <f t="shared" ref="F136:O136" si="94">IF(E135-F133&lt;=$E$130, F133-E135+$E$130,0)</f>
+        <f t="shared" ref="F136:O136" si="98">IF(E135-F133&lt;=$E$130, F133-E135+$E$130,0)</f>
         <v>0</v>
       </c>
       <c r="G136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>80</v>
       </c>
       <c r="H136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>220</v>
       </c>
       <c r="I136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>140</v>
       </c>
       <c r="J136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>100</v>
       </c>
       <c r="K136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>60</v>
       </c>
       <c r="L136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>50</v>
       </c>
       <c r="M136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>70</v>
       </c>
       <c r="N136" s="267">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>20</v>
       </c>
       <c r="O136" s="268">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
     </row>
@@ -39825,39 +39825,39 @@
         <v>0</v>
       </c>
       <c r="G137" s="267">
-        <f t="shared" ref="G137:O137" si="95" xml:space="preserve"> CEILING(G136/$E$129,1)*$E$129</f>
+        <f t="shared" ref="G137:O137" si="99" xml:space="preserve"> CEILING(G136/$E$129,1)*$E$129</f>
         <v>100</v>
       </c>
-      <c r="H137" s="391">
-        <f t="shared" si="95"/>
+      <c r="H137" s="388">
+        <f t="shared" si="99"/>
         <v>250</v>
       </c>
       <c r="I137" s="267">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>150</v>
       </c>
       <c r="J137" s="267">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>100</v>
       </c>
       <c r="K137" s="267">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>100</v>
       </c>
       <c r="L137" s="267">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>50</v>
       </c>
       <c r="M137" s="267">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>100</v>
       </c>
       <c r="N137" s="267">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>50</v>
       </c>
       <c r="O137" s="268">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
     </row>
@@ -39865,110 +39865,110 @@
       <c r="D138" s="133" t="s">
         <v>225</v>
       </c>
-      <c r="E138" s="392"/>
-      <c r="F138" s="393">
+      <c r="E138" s="389"/>
+      <c r="F138" s="390">
         <f>G137</f>
         <v>100</v>
       </c>
-      <c r="G138" s="393">
+      <c r="G138" s="390">
         <f>H137</f>
         <v>250</v>
       </c>
-      <c r="H138" s="393">
-        <f t="shared" ref="H138:O138" si="96">I137</f>
+      <c r="H138" s="390">
+        <f t="shared" ref="H138:O138" si="100">I137</f>
         <v>150</v>
       </c>
-      <c r="I138" s="393">
-        <f t="shared" si="96"/>
+      <c r="I138" s="390">
+        <f t="shared" si="100"/>
         <v>100</v>
       </c>
-      <c r="J138" s="393">
-        <f t="shared" si="96"/>
+      <c r="J138" s="390">
+        <f t="shared" si="100"/>
         <v>100</v>
       </c>
-      <c r="K138" s="393">
-        <f t="shared" si="96"/>
+      <c r="K138" s="390">
+        <f t="shared" si="100"/>
         <v>50</v>
       </c>
-      <c r="L138" s="393">
-        <f t="shared" si="96"/>
+      <c r="L138" s="390">
+        <f t="shared" si="100"/>
         <v>100</v>
       </c>
-      <c r="M138" s="393">
-        <f t="shared" si="96"/>
+      <c r="M138" s="390">
+        <f t="shared" si="100"/>
         <v>50</v>
       </c>
-      <c r="N138" s="393">
-        <f t="shared" si="96"/>
-        <v>0</v>
-      </c>
-      <c r="O138" s="394">
-        <f t="shared" si="96"/>
+      <c r="N138" s="390">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="O138" s="391">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="P138" s="177"/>
     </row>
     <row r="139" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D139" s="387" t="s">
+      <c r="D139" s="384" t="s">
         <v>223</v>
       </c>
-      <c r="E139" s="388"/>
-      <c r="F139" s="389">
+      <c r="E139" s="385"/>
+      <c r="F139" s="386">
         <f>IF(F136&gt;$E$131,F136-$E$131,0)</f>
         <v>0</v>
       </c>
-      <c r="G139" s="389">
-        <f t="shared" ref="G139:O139" si="97">IF(G136&gt;$E$131,G136-$E$131,0)</f>
-        <v>0</v>
-      </c>
-      <c r="H139" s="389">
-        <f t="shared" si="97"/>
-        <v>20</v>
-      </c>
-      <c r="I139" s="389">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="J139" s="389">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="K139" s="389">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="L139" s="389">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="M139" s="389">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="N139" s="389">
-        <f t="shared" si="97"/>
-        <v>0</v>
-      </c>
-      <c r="O139" s="390">
-        <f t="shared" si="97"/>
+      <c r="G139" s="386">
+        <f t="shared" ref="G139:O139" si="101">IF(G136&gt;$E$131,G136-$E$131,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H139" s="386">
+        <f t="shared" si="101"/>
+        <v>20</v>
+      </c>
+      <c r="I139" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="J139" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="K139" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="L139" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M139" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="N139" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="O139" s="387">
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="P139" s="177"/>
     </row>
     <row r="140" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="H140" s="385"/>
-      <c r="I140" s="384"/>
+      <c r="H140" s="382"/>
+      <c r="I140" s="381"/>
     </row>
     <row r="141" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="H141" s="417">
+      <c r="H141" s="414">
         <f>MIN(H119,H78,H38)</f>
         <v>2755</v>
       </c>
-      <c r="I141" s="384"/>
+      <c r="I141" s="381"/>
     </row>
     <row r="142" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="H142" s="385"/>
-      <c r="I142" s="384"/>
+      <c r="H142" s="382"/>
+      <c r="I142" s="381"/>
     </row>
     <row r="143" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C143" s="157" t="s">
@@ -39991,7 +39991,7 @@
       </c>
     </row>
     <row r="147" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C147" s="386" t="s">
+      <c r="C147" s="383" t="s">
         <v>140</v>
       </c>
       <c r="D147" s="85" t="s">

</xml_diff>

<commit_message>
Complete demand centre 1
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A22966-4266-4B17-9544-14E067FF1359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC572F1-89F0-48DE-B7D4-4B25DF6F0210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="1980" yWindow="804" windowWidth="16824" windowHeight="10092" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32835,8 +32835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
   <dimension ref="A2:AI147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33528,7 +33528,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="334">
-        <f t="shared" si="9"/>
+        <f>G24*G20</f>
         <v>16880</v>
       </c>
       <c r="H25" s="334">

</xml_diff>

<commit_message>
Complete demand centre 2 and 3
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC572F1-89F0-48DE-B7D4-4B25DF6F0210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C7B81F-FE5D-4FC3-B504-EB9DF24E6864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="804" windowWidth="16824" windowHeight="10092" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3396,9 +3396,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="66" xfId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="20" borderId="68" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3441,9 +3438,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="66" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="68" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3470,6 +3464,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="66" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="70" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7561,19 +7561,19 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="415" t="s">
+      <c r="C3" s="413" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="416"/>
-      <c r="E3" s="416"/>
-      <c r="F3" s="416"/>
-      <c r="G3" s="416"/>
-      <c r="H3" s="416"/>
-      <c r="I3" s="416"/>
-      <c r="J3" s="416"/>
-      <c r="K3" s="416"/>
-      <c r="L3" s="416"/>
-      <c r="M3" s="417"/>
+      <c r="D3" s="414"/>
+      <c r="E3" s="414"/>
+      <c r="F3" s="414"/>
+      <c r="G3" s="414"/>
+      <c r="H3" s="414"/>
+      <c r="I3" s="414"/>
+      <c r="J3" s="414"/>
+      <c r="K3" s="414"/>
+      <c r="L3" s="414"/>
+      <c r="M3" s="415"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
@@ -7945,19 +7945,19 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="415" t="s">
+      <c r="C4" s="413" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="416"/>
-      <c r="E4" s="416"/>
-      <c r="F4" s="416"/>
-      <c r="G4" s="416"/>
-      <c r="H4" s="416"/>
-      <c r="I4" s="416"/>
-      <c r="J4" s="416"/>
-      <c r="K4" s="416"/>
-      <c r="L4" s="416"/>
-      <c r="M4" s="417"/>
+      <c r="D4" s="414"/>
+      <c r="E4" s="414"/>
+      <c r="F4" s="414"/>
+      <c r="G4" s="414"/>
+      <c r="H4" s="414"/>
+      <c r="I4" s="414"/>
+      <c r="J4" s="414"/>
+      <c r="K4" s="414"/>
+      <c r="L4" s="414"/>
+      <c r="M4" s="415"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -8587,19 +8587,19 @@
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="415" t="s">
+      <c r="C23" s="413" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="416"/>
-      <c r="E23" s="416"/>
-      <c r="F23" s="416"/>
-      <c r="G23" s="416"/>
-      <c r="H23" s="416"/>
-      <c r="I23" s="416"/>
-      <c r="J23" s="416"/>
-      <c r="K23" s="416"/>
-      <c r="L23" s="416"/>
-      <c r="M23" s="417"/>
+      <c r="D23" s="414"/>
+      <c r="E23" s="414"/>
+      <c r="F23" s="414"/>
+      <c r="G23" s="414"/>
+      <c r="H23" s="414"/>
+      <c r="I23" s="414"/>
+      <c r="J23" s="414"/>
+      <c r="K23" s="414"/>
+      <c r="L23" s="414"/>
+      <c r="M23" s="415"/>
       <c r="O23" s="24" t="s">
         <v>68</v>
       </c>
@@ -10642,17 +10642,17 @@
       <c r="C51" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="416" t="s">
+      <c r="D51" s="414" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="416"/>
-      <c r="F51" s="416"/>
-      <c r="G51" s="416"/>
-      <c r="H51" s="416"/>
-      <c r="I51" s="416"/>
-      <c r="J51" s="416"/>
-      <c r="K51" s="416"/>
-      <c r="L51" s="417"/>
+      <c r="E51" s="414"/>
+      <c r="F51" s="414"/>
+      <c r="G51" s="414"/>
+      <c r="H51" s="414"/>
+      <c r="I51" s="414"/>
+      <c r="J51" s="414"/>
+      <c r="K51" s="414"/>
+      <c r="L51" s="415"/>
       <c r="M51"/>
       <c r="N51"/>
       <c r="O51"/>
@@ -32835,8 +32835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
   <dimension ref="A2:AI147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="D76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32979,7 +32979,7 @@
       <c r="O10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="406" t="s">
+      <c r="P10" s="405" t="s">
         <v>226</v>
       </c>
     </row>
@@ -32988,22 +32988,22 @@
         <v>162</v>
       </c>
       <c r="E11" s="276"/>
-      <c r="F11" s="393"/>
-      <c r="G11" s="393"/>
-      <c r="H11" s="393"/>
-      <c r="I11" s="393">
+      <c r="F11" s="392"/>
+      <c r="G11" s="392"/>
+      <c r="H11" s="392"/>
+      <c r="I11" s="392">
         <v>30</v>
       </c>
-      <c r="J11" s="408">
+      <c r="J11" s="406">
         <v>40</v>
       </c>
-      <c r="K11" s="393">
+      <c r="K11" s="392">
         <v>15</v>
       </c>
-      <c r="L11" s="393"/>
-      <c r="M11" s="393"/>
-      <c r="N11" s="393"/>
-      <c r="O11" s="394">
+      <c r="L11" s="392"/>
+      <c r="M11" s="392"/>
+      <c r="N11" s="392"/>
+      <c r="O11" s="393">
         <v>10</v>
       </c>
       <c r="P11" s="191" t="s">
@@ -33018,46 +33018,46 @@
         <v>204</v>
       </c>
       <c r="E12" s="278"/>
-      <c r="F12" s="395">
+      <c r="F12" s="394">
         <v>40</v>
       </c>
-      <c r="G12" s="395">
+      <c r="G12" s="394">
         <v>30</v>
       </c>
-      <c r="H12" s="395"/>
-      <c r="I12" s="395"/>
-      <c r="J12" s="395"/>
-      <c r="K12" s="395"/>
-      <c r="L12" s="395"/>
-      <c r="M12" s="395"/>
-      <c r="N12" s="395"/>
-      <c r="O12" s="396"/>
+      <c r="H12" s="394"/>
+      <c r="I12" s="394"/>
+      <c r="J12" s="394"/>
+      <c r="K12" s="394"/>
+      <c r="L12" s="394"/>
+      <c r="M12" s="394"/>
+      <c r="N12" s="394"/>
+      <c r="O12" s="395"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D13" s="279" t="s">
         <v>165</v>
       </c>
       <c r="E13" s="280"/>
-      <c r="F13" s="395"/>
-      <c r="G13" s="395"/>
-      <c r="H13" s="395">
-        <v>20</v>
-      </c>
-      <c r="I13" s="395">
+      <c r="F13" s="394"/>
+      <c r="G13" s="394"/>
+      <c r="H13" s="394">
+        <v>20</v>
+      </c>
+      <c r="I13" s="394">
         <v>50</v>
       </c>
-      <c r="J13" s="395">
+      <c r="J13" s="394">
         <v>60</v>
       </c>
-      <c r="K13" s="395"/>
-      <c r="L13" s="395">
+      <c r="K13" s="394"/>
+      <c r="L13" s="394">
         <v>40</v>
       </c>
-      <c r="M13" s="395"/>
-      <c r="N13" s="395">
+      <c r="M13" s="394"/>
+      <c r="N13" s="394">
         <v>40</v>
       </c>
-      <c r="O13" s="396"/>
+      <c r="O13" s="395"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14" s="251" t="s">
@@ -33067,20 +33067,20 @@
         <v>205</v>
       </c>
       <c r="E14" s="284"/>
-      <c r="F14" s="395">
+      <c r="F14" s="394">
         <v>50</v>
       </c>
-      <c r="G14" s="395">
+      <c r="G14" s="394">
         <v>40</v>
       </c>
-      <c r="H14" s="395"/>
-      <c r="I14" s="395"/>
-      <c r="J14" s="395"/>
-      <c r="K14" s="395"/>
-      <c r="L14" s="395"/>
-      <c r="M14" s="395"/>
-      <c r="N14" s="395"/>
-      <c r="O14" s="396"/>
+      <c r="H14" s="394"/>
+      <c r="I14" s="394"/>
+      <c r="J14" s="394"/>
+      <c r="K14" s="394"/>
+      <c r="L14" s="394"/>
+      <c r="M14" s="394"/>
+      <c r="N14" s="394"/>
+      <c r="O14" s="395"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="287" t="s">
@@ -33133,10 +33133,10 @@
         <v>203</v>
       </c>
       <c r="E16" s="263"/>
-      <c r="F16" s="399">
+      <c r="F16" s="398">
         <v>80</v>
       </c>
-      <c r="G16" s="399">
+      <c r="G16" s="398">
         <v>80</v>
       </c>
       <c r="H16" s="264"/>
@@ -33155,7 +33155,7 @@
       <c r="D17" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="E17" s="400">
+      <c r="E17" s="399">
         <v>50</v>
       </c>
       <c r="F17" s="267">
@@ -33484,34 +33484,34 @@
         <v>170</v>
       </c>
       <c r="E24" s="233"/>
-      <c r="F24" s="397">
+      <c r="F24" s="396">
         <v>210</v>
       </c>
-      <c r="G24" s="397">
+      <c r="G24" s="396">
         <v>211</v>
       </c>
-      <c r="H24" s="397">
+      <c r="H24" s="396">
         <v>213</v>
       </c>
-      <c r="I24" s="397">
+      <c r="I24" s="396">
         <v>215</v>
       </c>
-      <c r="J24" s="397">
+      <c r="J24" s="396">
         <v>215</v>
       </c>
-      <c r="K24" s="397">
+      <c r="K24" s="396">
         <v>216</v>
       </c>
-      <c r="L24" s="397">
+      <c r="L24" s="396">
         <v>214</v>
       </c>
-      <c r="M24" s="397">
+      <c r="M24" s="396">
         <v>212</v>
       </c>
-      <c r="N24" s="397">
+      <c r="N24" s="396">
         <v>210</v>
       </c>
-      <c r="O24" s="398">
+      <c r="O24" s="397">
         <v>209</v>
       </c>
     </row>
@@ -33627,34 +33627,34 @@
         <v>173</v>
       </c>
       <c r="E27" s="273"/>
-      <c r="F27" s="397">
+      <c r="F27" s="396">
         <v>410</v>
       </c>
-      <c r="G27" s="397">
+      <c r="G27" s="396">
         <v>413</v>
       </c>
-      <c r="H27" s="397">
+      <c r="H27" s="396">
         <v>410</v>
       </c>
-      <c r="I27" s="397">
+      <c r="I27" s="396">
         <v>415</v>
       </c>
-      <c r="J27" s="397">
+      <c r="J27" s="396">
         <v>418</v>
       </c>
-      <c r="K27" s="397">
+      <c r="K27" s="396">
         <v>430</v>
       </c>
-      <c r="L27" s="397">
+      <c r="L27" s="396">
         <v>423</v>
       </c>
-      <c r="M27" s="397">
+      <c r="M27" s="396">
         <v>419</v>
       </c>
-      <c r="N27" s="397">
+      <c r="N27" s="396">
         <v>417</v>
       </c>
-      <c r="O27" s="398">
+      <c r="O27" s="397">
         <v>422</v>
       </c>
     </row>
@@ -33862,7 +33862,7 @@
       </c>
       <c r="P31" s="251"/>
       <c r="AC31" s="6"/>
-      <c r="AD31" s="413"/>
+      <c r="AD31" s="411"/>
       <c r="AF31" s="349"/>
       <c r="AH31" s="349"/>
     </row>
@@ -35396,7 +35396,7 @@
       <c r="F51" s="392"/>
       <c r="G51" s="392"/>
       <c r="H51" s="392"/>
-      <c r="I51" s="407">
+      <c r="I51" s="406">
         <v>20</v>
       </c>
       <c r="J51" s="392">
@@ -35410,7 +35410,7 @@
         <v>10</v>
       </c>
       <c r="N51" s="392"/>
-      <c r="O51" s="392">
+      <c r="O51" s="393">
         <v>10</v>
       </c>
       <c r="S51" s="138"/>
@@ -35468,18 +35468,18 @@
         <v>204</v>
       </c>
       <c r="E52" s="278"/>
-      <c r="F52" s="392"/>
-      <c r="G52" s="392">
+      <c r="F52" s="394"/>
+      <c r="G52" s="394">
         <v>10</v>
       </c>
-      <c r="H52" s="392"/>
-      <c r="I52" s="392"/>
-      <c r="J52" s="392"/>
-      <c r="K52" s="392"/>
-      <c r="L52" s="392"/>
-      <c r="M52" s="392"/>
-      <c r="N52" s="392"/>
-      <c r="O52" s="392"/>
+      <c r="H52" s="394"/>
+      <c r="I52" s="394"/>
+      <c r="J52" s="394"/>
+      <c r="K52" s="394"/>
+      <c r="L52" s="394"/>
+      <c r="M52" s="394"/>
+      <c r="N52" s="394"/>
+      <c r="O52" s="395"/>
       <c r="S52" s="138"/>
       <c r="T52" s="138"/>
       <c r="V52" s="138">
@@ -35535,24 +35535,24 @@
         <v>165</v>
       </c>
       <c r="E53" s="280"/>
-      <c r="F53" s="392"/>
-      <c r="G53" s="392"/>
-      <c r="H53" s="392"/>
-      <c r="I53" s="392">
+      <c r="F53" s="394"/>
+      <c r="G53" s="394"/>
+      <c r="H53" s="394"/>
+      <c r="I53" s="394">
         <v>60</v>
       </c>
-      <c r="J53" s="392">
+      <c r="J53" s="394">
         <v>80</v>
       </c>
-      <c r="K53" s="392"/>
-      <c r="L53" s="392">
+      <c r="K53" s="394"/>
+      <c r="L53" s="394">
         <v>40</v>
       </c>
-      <c r="M53" s="392"/>
-      <c r="N53" s="392">
+      <c r="M53" s="394"/>
+      <c r="N53" s="394">
         <v>50</v>
       </c>
-      <c r="O53" s="392"/>
+      <c r="O53" s="395"/>
       <c r="S53" s="138"/>
       <c r="T53" s="138"/>
       <c r="V53" s="138">
@@ -35608,18 +35608,18 @@
         <v>205</v>
       </c>
       <c r="E54" s="284"/>
-      <c r="F54" s="392"/>
-      <c r="G54" s="392">
+      <c r="F54" s="394"/>
+      <c r="G54" s="394">
         <v>40</v>
       </c>
-      <c r="H54" s="392"/>
-      <c r="I54" s="392"/>
-      <c r="J54" s="392"/>
-      <c r="K54" s="392"/>
-      <c r="L54" s="392"/>
-      <c r="M54" s="392"/>
-      <c r="N54" s="392"/>
-      <c r="O54" s="392"/>
+      <c r="H54" s="394"/>
+      <c r="I54" s="394"/>
+      <c r="J54" s="394"/>
+      <c r="K54" s="394"/>
+      <c r="L54" s="394"/>
+      <c r="M54" s="394"/>
+      <c r="N54" s="394"/>
+      <c r="O54" s="395"/>
       <c r="S54" s="138"/>
       <c r="T54" s="138"/>
       <c r="V54" s="138">
@@ -35770,10 +35770,10 @@
         <v>203</v>
       </c>
       <c r="E56" s="263"/>
-      <c r="F56" s="399">
-        <v>20</v>
-      </c>
-      <c r="G56" s="399"/>
+      <c r="F56" s="398">
+        <v>20</v>
+      </c>
+      <c r="G56" s="398"/>
       <c r="H56" s="264"/>
       <c r="I56" s="264"/>
       <c r="J56" s="264"/>
@@ -35834,7 +35834,7 @@
       <c r="D57" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="E57" s="400">
+      <c r="E57" s="399">
         <v>30</v>
       </c>
       <c r="F57" s="267">
@@ -36478,38 +36478,38 @@
       </c>
     </row>
     <row r="64" spans="3:34" x14ac:dyDescent="0.3">
-      <c r="D64" s="401" t="s">
+      <c r="D64" s="400" t="s">
         <v>170</v>
       </c>
       <c r="E64" s="233"/>
-      <c r="F64" s="404">
+      <c r="F64" s="403">
         <v>210</v>
       </c>
-      <c r="G64" s="404">
+      <c r="G64" s="403">
         <v>211</v>
       </c>
-      <c r="H64" s="404">
+      <c r="H64" s="403">
         <v>213</v>
       </c>
-      <c r="I64" s="404">
+      <c r="I64" s="403">
         <v>215</v>
       </c>
-      <c r="J64" s="404">
+      <c r="J64" s="403">
         <v>215</v>
       </c>
-      <c r="K64" s="404">
+      <c r="K64" s="403">
         <v>216</v>
       </c>
-      <c r="L64" s="404">
+      <c r="L64" s="403">
         <v>214</v>
       </c>
-      <c r="M64" s="404">
+      <c r="M64" s="403">
         <v>212</v>
       </c>
-      <c r="N64" s="404">
+      <c r="N64" s="403">
         <v>210</v>
       </c>
-      <c r="O64" s="405">
+      <c r="O64" s="404">
         <v>209</v>
       </c>
       <c r="W64" s="138">
@@ -36560,7 +36560,7 @@
       <c r="C65" s="251" t="s">
         <v>181</v>
       </c>
-      <c r="D65" s="402" t="s">
+      <c r="D65" s="401" t="s">
         <v>171</v>
       </c>
       <c r="E65" s="243"/>
@@ -36652,7 +36652,7 @@
       </c>
     </row>
     <row r="66" spans="3:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D66" s="403" t="s">
+      <c r="D66" s="402" t="s">
         <v>172</v>
       </c>
       <c r="E66" s="255"/>
@@ -36748,34 +36748,34 @@
         <v>173</v>
       </c>
       <c r="E67" s="273"/>
-      <c r="F67" s="397">
+      <c r="F67" s="396">
         <v>411</v>
       </c>
-      <c r="G67" s="397">
+      <c r="G67" s="396">
         <v>414</v>
       </c>
-      <c r="H67" s="397">
+      <c r="H67" s="396">
         <v>412</v>
       </c>
-      <c r="I67" s="397">
+      <c r="I67" s="396">
         <v>413</v>
       </c>
-      <c r="J67" s="397">
+      <c r="J67" s="396">
         <v>418</v>
       </c>
-      <c r="K67" s="397">
+      <c r="K67" s="396">
         <v>428</v>
       </c>
-      <c r="L67" s="397">
+      <c r="L67" s="396">
         <v>426</v>
       </c>
-      <c r="M67" s="397">
+      <c r="M67" s="396">
         <v>419</v>
       </c>
-      <c r="N67" s="397">
+      <c r="N67" s="396">
         <v>415</v>
       </c>
-      <c r="O67" s="398">
+      <c r="O67" s="397">
         <v>421</v>
       </c>
       <c r="W67" s="138">
@@ -37007,47 +37007,47 @@
       </c>
     </row>
     <row r="70" spans="3:35" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D70" s="409" t="s">
+      <c r="D70" s="407" t="s">
         <v>193</v>
       </c>
-      <c r="E70" s="410"/>
-      <c r="F70" s="411">
+      <c r="E70" s="408"/>
+      <c r="F70" s="409">
         <f>SUM(G51:G52)</f>
         <v>10</v>
       </c>
-      <c r="G70" s="411">
+      <c r="G70" s="409">
         <f t="shared" ref="G70:O70" si="46">SUM(H51:H52)</f>
         <v>0</v>
       </c>
-      <c r="H70" s="411">
+      <c r="H70" s="409">
         <f t="shared" si="46"/>
         <v>20</v>
       </c>
-      <c r="I70" s="411">
+      <c r="I70" s="409">
         <f t="shared" si="46"/>
         <v>20</v>
       </c>
-      <c r="J70" s="411">
+      <c r="J70" s="409">
         <f t="shared" si="46"/>
         <v>15</v>
       </c>
-      <c r="K70" s="411">
+      <c r="K70" s="409">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="L70" s="411">
+      <c r="L70" s="409">
         <f t="shared" si="46"/>
         <v>10</v>
       </c>
-      <c r="M70" s="411">
+      <c r="M70" s="409">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="N70" s="411">
+      <c r="N70" s="409">
         <f t="shared" si="46"/>
         <v>10</v>
       </c>
-      <c r="O70" s="412">
+      <c r="O70" s="410">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -38067,24 +38067,24 @@
         <v>162</v>
       </c>
       <c r="E92" s="276"/>
-      <c r="F92" s="302"/>
-      <c r="G92" s="302"/>
-      <c r="H92" s="158">
+      <c r="F92" s="416"/>
+      <c r="G92" s="416"/>
+      <c r="H92" s="416">
         <v>15</v>
       </c>
-      <c r="I92" s="303">
-        <v>20</v>
-      </c>
-      <c r="J92" s="303">
+      <c r="I92" s="416">
+        <v>20</v>
+      </c>
+      <c r="J92" s="416">
         <v>10</v>
       </c>
-      <c r="K92" s="302"/>
-      <c r="L92" s="302"/>
-      <c r="M92" s="302">
+      <c r="K92" s="416"/>
+      <c r="L92" s="416"/>
+      <c r="M92" s="416">
         <v>15</v>
       </c>
-      <c r="N92" s="302"/>
-      <c r="O92" s="304">
+      <c r="N92" s="416"/>
+      <c r="O92" s="417">
         <v>0</v>
       </c>
       <c r="S92" s="138"/>
@@ -38095,18 +38095,18 @@
         <v>204</v>
       </c>
       <c r="E93" s="278"/>
-      <c r="F93" s="301">
+      <c r="F93" s="416">
         <v>10</v>
       </c>
-      <c r="G93" s="301"/>
-      <c r="H93" s="301"/>
-      <c r="I93" s="305"/>
-      <c r="J93" s="305"/>
-      <c r="K93" s="301"/>
-      <c r="L93" s="301"/>
-      <c r="M93" s="301"/>
-      <c r="N93" s="301"/>
-      <c r="O93" s="306"/>
+      <c r="G93" s="416"/>
+      <c r="H93" s="416"/>
+      <c r="I93" s="416"/>
+      <c r="J93" s="416"/>
+      <c r="K93" s="416"/>
+      <c r="L93" s="416"/>
+      <c r="M93" s="416"/>
+      <c r="N93" s="416"/>
+      <c r="O93" s="417"/>
       <c r="S93" s="138"/>
       <c r="T93" s="138"/>
     </row>
@@ -38115,28 +38115,28 @@
         <v>165</v>
       </c>
       <c r="E94" s="280"/>
-      <c r="F94" s="281"/>
-      <c r="G94" s="281"/>
-      <c r="H94" s="281">
+      <c r="F94" s="416"/>
+      <c r="G94" s="416"/>
+      <c r="H94" s="416">
         <v>40</v>
       </c>
-      <c r="I94" s="281">
+      <c r="I94" s="416">
         <v>30</v>
       </c>
-      <c r="J94" s="281">
+      <c r="J94" s="416">
         <v>40</v>
       </c>
-      <c r="K94" s="281">
-        <v>20</v>
-      </c>
-      <c r="L94" s="281">
+      <c r="K94" s="416">
+        <v>20</v>
+      </c>
+      <c r="L94" s="416">
         <v>30</v>
       </c>
-      <c r="M94" s="281"/>
-      <c r="N94" s="281">
+      <c r="M94" s="416"/>
+      <c r="N94" s="416">
         <v>30</v>
       </c>
-      <c r="O94" s="282">
+      <c r="O94" s="417">
         <v>20</v>
       </c>
       <c r="S94" s="138"/>
@@ -38147,18 +38147,18 @@
         <v>205</v>
       </c>
       <c r="E95" s="284"/>
-      <c r="F95" s="285"/>
-      <c r="G95" s="285">
-        <v>20</v>
-      </c>
-      <c r="H95" s="285"/>
-      <c r="I95" s="285"/>
-      <c r="J95" s="285"/>
-      <c r="K95" s="285"/>
-      <c r="L95" s="285"/>
-      <c r="M95" s="285"/>
-      <c r="N95" s="285"/>
-      <c r="O95" s="286"/>
+      <c r="F95" s="416"/>
+      <c r="G95" s="416">
+        <v>20</v>
+      </c>
+      <c r="H95" s="416"/>
+      <c r="I95" s="416"/>
+      <c r="J95" s="416"/>
+      <c r="K95" s="416"/>
+      <c r="L95" s="416"/>
+      <c r="M95" s="416"/>
+      <c r="N95" s="416"/>
+      <c r="O95" s="417"/>
       <c r="S95" s="138"/>
       <c r="T95" s="138"/>
     </row>
@@ -38212,8 +38212,8 @@
       <c r="D97" s="175" t="s">
         <v>203</v>
       </c>
-      <c r="E97" s="169"/>
-      <c r="F97" s="98">
+      <c r="E97" s="263"/>
+      <c r="F97" s="398">
         <v>20</v>
       </c>
       <c r="G97" s="98"/>
@@ -38230,10 +38230,10 @@
       <c r="D98" s="131" t="s">
         <v>202</v>
       </c>
-      <c r="E98" s="170">
-        <v>20</v>
-      </c>
-      <c r="F98" s="97">
+      <c r="E98" s="399">
+        <v>20</v>
+      </c>
+      <c r="F98" s="267">
         <f>E98+F97+F100-F96</f>
         <v>30</v>
       </c>
@@ -38562,34 +38562,34 @@
         <v>170</v>
       </c>
       <c r="E105" s="233"/>
-      <c r="F105" s="181">
+      <c r="F105" s="396">
         <v>210</v>
       </c>
-      <c r="G105" s="181">
+      <c r="G105" s="396">
         <v>211</v>
       </c>
-      <c r="H105" s="181">
+      <c r="H105" s="396">
         <v>213</v>
       </c>
-      <c r="I105" s="181">
+      <c r="I105" s="396">
         <v>215</v>
       </c>
-      <c r="J105" s="181">
+      <c r="J105" s="396">
         <v>215</v>
       </c>
-      <c r="K105" s="181">
+      <c r="K105" s="396">
         <v>216</v>
       </c>
-      <c r="L105" s="181">
+      <c r="L105" s="396">
         <v>214</v>
       </c>
-      <c r="M105" s="181">
+      <c r="M105" s="396">
         <v>212</v>
       </c>
-      <c r="N105" s="181">
+      <c r="N105" s="396">
         <v>210</v>
       </c>
-      <c r="O105" s="182">
+      <c r="O105" s="397">
         <v>209</v>
       </c>
     </row>
@@ -38699,34 +38699,34 @@
         <v>173</v>
       </c>
       <c r="E108" s="273"/>
-      <c r="F108" s="181">
+      <c r="F108" s="396">
         <v>410</v>
       </c>
-      <c r="G108" s="181">
+      <c r="G108" s="396">
         <v>413</v>
       </c>
-      <c r="H108" s="181">
+      <c r="H108" s="396">
         <v>410</v>
       </c>
-      <c r="I108" s="181">
+      <c r="I108" s="396">
         <v>415</v>
       </c>
-      <c r="J108" s="181">
+      <c r="J108" s="396">
         <v>418</v>
       </c>
-      <c r="K108" s="181">
+      <c r="K108" s="396">
         <v>430</v>
       </c>
-      <c r="L108" s="181">
+      <c r="L108" s="396">
         <v>423</v>
       </c>
-      <c r="M108" s="181">
+      <c r="M108" s="396">
         <v>419</v>
       </c>
-      <c r="N108" s="181">
+      <c r="N108" s="396">
         <v>417</v>
       </c>
-      <c r="O108" s="182">
+      <c r="O108" s="397">
         <v>422</v>
       </c>
     </row>
@@ -38829,47 +38829,47 @@
       </c>
     </row>
     <row r="111" spans="3:35" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D111" s="409" t="s">
+      <c r="D111" s="407" t="s">
         <v>193</v>
       </c>
-      <c r="E111" s="410"/>
-      <c r="F111" s="411">
+      <c r="E111" s="408"/>
+      <c r="F111" s="409">
         <f>SUM(F92:F93)</f>
         <v>10</v>
       </c>
-      <c r="G111" s="411">
+      <c r="G111" s="409">
         <f t="shared" ref="G111:O111" si="71">SUM(G92:G93)</f>
         <v>0</v>
       </c>
-      <c r="H111" s="411">
+      <c r="H111" s="409">
         <f t="shared" si="71"/>
         <v>15</v>
       </c>
-      <c r="I111" s="411">
+      <c r="I111" s="409">
         <f t="shared" si="71"/>
         <v>20</v>
       </c>
-      <c r="J111" s="411">
+      <c r="J111" s="409">
         <f t="shared" si="71"/>
         <v>10</v>
       </c>
-      <c r="K111" s="411">
+      <c r="K111" s="409">
         <f t="shared" si="71"/>
         <v>0</v>
       </c>
-      <c r="L111" s="411">
+      <c r="L111" s="409">
         <f t="shared" si="71"/>
         <v>0</v>
       </c>
-      <c r="M111" s="411">
+      <c r="M111" s="409">
         <f t="shared" si="71"/>
         <v>15</v>
       </c>
-      <c r="N111" s="411">
+      <c r="N111" s="409">
         <f t="shared" si="71"/>
         <v>0</v>
       </c>
-      <c r="O111" s="412">
+      <c r="O111" s="410">
         <f t="shared" si="71"/>
         <v>0</v>
       </c>
@@ -39960,7 +39960,7 @@
       <c r="I140" s="381"/>
     </row>
     <row r="141" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="H141" s="414">
+      <c r="H141" s="412">
         <f>MIN(H119,H78,H38)</f>
         <v>2755</v>
       </c>

</xml_diff>

<commit_message>
added profit loss each DC
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C7B81F-FE5D-4FC3-B504-EB9DF24E6864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E16285-9318-4848-B068-4C7D2358A303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="28680" yWindow="240" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="232">
   <si>
     <t>week</t>
   </si>
@@ -1121,6 +1121,9 @@
   </si>
   <si>
     <t>(Term Only) Final profit</t>
+  </si>
+  <si>
+    <t>Supplier Forecasted DEMAND</t>
   </si>
 </sst>
 </file>
@@ -3457,6 +3460,12 @@
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="66" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="70" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3464,12 +3473,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="66" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="70" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7561,19 +7564,19 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="413" t="s">
+      <c r="C3" s="415" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="414"/>
-      <c r="E3" s="414"/>
-      <c r="F3" s="414"/>
-      <c r="G3" s="414"/>
-      <c r="H3" s="414"/>
-      <c r="I3" s="414"/>
-      <c r="J3" s="414"/>
-      <c r="K3" s="414"/>
-      <c r="L3" s="414"/>
-      <c r="M3" s="415"/>
+      <c r="D3" s="416"/>
+      <c r="E3" s="416"/>
+      <c r="F3" s="416"/>
+      <c r="G3" s="416"/>
+      <c r="H3" s="416"/>
+      <c r="I3" s="416"/>
+      <c r="J3" s="416"/>
+      <c r="K3" s="416"/>
+      <c r="L3" s="416"/>
+      <c r="M3" s="417"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
@@ -7945,19 +7948,19 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="413" t="s">
+      <c r="C4" s="415" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="414"/>
-      <c r="E4" s="414"/>
-      <c r="F4" s="414"/>
-      <c r="G4" s="414"/>
-      <c r="H4" s="414"/>
-      <c r="I4" s="414"/>
-      <c r="J4" s="414"/>
-      <c r="K4" s="414"/>
-      <c r="L4" s="414"/>
-      <c r="M4" s="415"/>
+      <c r="D4" s="416"/>
+      <c r="E4" s="416"/>
+      <c r="F4" s="416"/>
+      <c r="G4" s="416"/>
+      <c r="H4" s="416"/>
+      <c r="I4" s="416"/>
+      <c r="J4" s="416"/>
+      <c r="K4" s="416"/>
+      <c r="L4" s="416"/>
+      <c r="M4" s="417"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -8587,19 +8590,19 @@
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="413" t="s">
+      <c r="C23" s="415" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="414"/>
-      <c r="E23" s="414"/>
-      <c r="F23" s="414"/>
-      <c r="G23" s="414"/>
-      <c r="H23" s="414"/>
-      <c r="I23" s="414"/>
-      <c r="J23" s="414"/>
-      <c r="K23" s="414"/>
-      <c r="L23" s="414"/>
-      <c r="M23" s="415"/>
+      <c r="D23" s="416"/>
+      <c r="E23" s="416"/>
+      <c r="F23" s="416"/>
+      <c r="G23" s="416"/>
+      <c r="H23" s="416"/>
+      <c r="I23" s="416"/>
+      <c r="J23" s="416"/>
+      <c r="K23" s="416"/>
+      <c r="L23" s="416"/>
+      <c r="M23" s="417"/>
       <c r="O23" s="24" t="s">
         <v>68</v>
       </c>
@@ -10642,17 +10645,17 @@
       <c r="C51" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="414" t="s">
+      <c r="D51" s="416" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="414"/>
-      <c r="F51" s="414"/>
-      <c r="G51" s="414"/>
-      <c r="H51" s="414"/>
-      <c r="I51" s="414"/>
-      <c r="J51" s="414"/>
-      <c r="K51" s="414"/>
-      <c r="L51" s="415"/>
+      <c r="E51" s="416"/>
+      <c r="F51" s="416"/>
+      <c r="G51" s="416"/>
+      <c r="H51" s="416"/>
+      <c r="I51" s="416"/>
+      <c r="J51" s="416"/>
+      <c r="K51" s="416"/>
+      <c r="L51" s="417"/>
       <c r="M51"/>
       <c r="N51"/>
       <c r="O51"/>
@@ -32835,8 +32838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
   <dimension ref="A2:AI147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M90" sqref="M90"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33766,11 +33769,11 @@
         <v>0</v>
       </c>
       <c r="G30" s="258">
-        <f t="shared" ref="G30:O30" si="13">SUM(I11:I12)</f>
+        <f>SUM(I11:I12)</f>
         <v>30</v>
       </c>
       <c r="H30" s="258">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="G30:O30" si="13">SUM(J11:J12)</f>
         <v>40</v>
       </c>
       <c r="I30" s="258">
@@ -33821,15 +33824,15 @@
       </c>
       <c r="E31" s="307"/>
       <c r="F31" s="258">
-        <f>F139</f>
+        <f>MIN(F139,F30)</f>
         <v>0</v>
       </c>
       <c r="G31" s="258">
-        <f>G139</f>
+        <f t="shared" ref="G31:O31" si="14">MIN(G139,G30)</f>
         <v>0</v>
       </c>
       <c r="H31" s="258">
-        <f t="shared" ref="H31:O31" si="14">H139</f>
+        <f t="shared" si="14"/>
         <v>20</v>
       </c>
       <c r="I31" s="258">
@@ -37104,11 +37107,11 @@
       </c>
       <c r="E71" s="307"/>
       <c r="F71" s="258">
-        <f>F139</f>
+        <f>MIN(F139,F70)</f>
         <v>0</v>
       </c>
       <c r="G71" s="258">
-        <f t="shared" ref="G71:O71" si="47">G139</f>
+        <f t="shared" ref="G71:O71" si="47">MIN(G139,G70)</f>
         <v>0</v>
       </c>
       <c r="H71" s="258">
@@ -38067,24 +38070,24 @@
         <v>162</v>
       </c>
       <c r="E92" s="276"/>
-      <c r="F92" s="416"/>
-      <c r="G92" s="416"/>
-      <c r="H92" s="416">
+      <c r="F92" s="413"/>
+      <c r="G92" s="413"/>
+      <c r="H92" s="413">
         <v>15</v>
       </c>
-      <c r="I92" s="416">
-        <v>20</v>
-      </c>
-      <c r="J92" s="416">
+      <c r="I92" s="413">
+        <v>20</v>
+      </c>
+      <c r="J92" s="413">
         <v>10</v>
       </c>
-      <c r="K92" s="416"/>
-      <c r="L92" s="416"/>
-      <c r="M92" s="416">
+      <c r="K92" s="413"/>
+      <c r="L92" s="413"/>
+      <c r="M92" s="413">
         <v>15</v>
       </c>
-      <c r="N92" s="416"/>
-      <c r="O92" s="417">
+      <c r="N92" s="413"/>
+      <c r="O92" s="414">
         <v>0</v>
       </c>
       <c r="S92" s="138"/>
@@ -38095,18 +38098,18 @@
         <v>204</v>
       </c>
       <c r="E93" s="278"/>
-      <c r="F93" s="416">
+      <c r="F93" s="413">
         <v>10</v>
       </c>
-      <c r="G93" s="416"/>
-      <c r="H93" s="416"/>
-      <c r="I93" s="416"/>
-      <c r="J93" s="416"/>
-      <c r="K93" s="416"/>
-      <c r="L93" s="416"/>
-      <c r="M93" s="416"/>
-      <c r="N93" s="416"/>
-      <c r="O93" s="417"/>
+      <c r="G93" s="413"/>
+      <c r="H93" s="413"/>
+      <c r="I93" s="413"/>
+      <c r="J93" s="413"/>
+      <c r="K93" s="413"/>
+      <c r="L93" s="413"/>
+      <c r="M93" s="413"/>
+      <c r="N93" s="413"/>
+      <c r="O93" s="414"/>
       <c r="S93" s="138"/>
       <c r="T93" s="138"/>
     </row>
@@ -38115,28 +38118,28 @@
         <v>165</v>
       </c>
       <c r="E94" s="280"/>
-      <c r="F94" s="416"/>
-      <c r="G94" s="416"/>
-      <c r="H94" s="416">
+      <c r="F94" s="413"/>
+      <c r="G94" s="413"/>
+      <c r="H94" s="413">
         <v>40</v>
       </c>
-      <c r="I94" s="416">
+      <c r="I94" s="413">
         <v>30</v>
       </c>
-      <c r="J94" s="416">
+      <c r="J94" s="413">
         <v>40</v>
       </c>
-      <c r="K94" s="416">
-        <v>20</v>
-      </c>
-      <c r="L94" s="416">
+      <c r="K94" s="413">
+        <v>20</v>
+      </c>
+      <c r="L94" s="413">
         <v>30</v>
       </c>
-      <c r="M94" s="416"/>
-      <c r="N94" s="416">
+      <c r="M94" s="413"/>
+      <c r="N94" s="413">
         <v>30</v>
       </c>
-      <c r="O94" s="417">
+      <c r="O94" s="414">
         <v>20</v>
       </c>
       <c r="S94" s="138"/>
@@ -38147,18 +38150,18 @@
         <v>205</v>
       </c>
       <c r="E95" s="284"/>
-      <c r="F95" s="416"/>
-      <c r="G95" s="416">
-        <v>20</v>
-      </c>
-      <c r="H95" s="416"/>
-      <c r="I95" s="416"/>
-      <c r="J95" s="416"/>
-      <c r="K95" s="416"/>
-      <c r="L95" s="416"/>
-      <c r="M95" s="416"/>
-      <c r="N95" s="416"/>
-      <c r="O95" s="417"/>
+      <c r="F95" s="413"/>
+      <c r="G95" s="413">
+        <v>20</v>
+      </c>
+      <c r="H95" s="413"/>
+      <c r="I95" s="413"/>
+      <c r="J95" s="413"/>
+      <c r="K95" s="413"/>
+      <c r="L95" s="413"/>
+      <c r="M95" s="413"/>
+      <c r="N95" s="413"/>
+      <c r="O95" s="414"/>
       <c r="S95" s="138"/>
       <c r="T95" s="138"/>
     </row>
@@ -38432,7 +38435,7 @@
         <v>0</v>
       </c>
       <c r="H102" s="370">
-        <f t="shared" si="64"/>
+        <f>QUOTIENT(MOD(H101+$E$87-1,$E$86),$E$87)</f>
         <v>0</v>
       </c>
       <c r="I102" s="370">
@@ -39661,7 +39664,7 @@
     </row>
     <row r="133" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D133" s="129" t="s">
-        <v>104</v>
+        <v>231</v>
       </c>
       <c r="E133" s="115"/>
       <c r="F133" s="136">
@@ -39922,7 +39925,7 @@
         <v>0</v>
       </c>
       <c r="H139" s="386">
-        <f t="shared" si="101"/>
+        <f>IF(H136&gt;$E$131,H136-$E$131,0)</f>
         <v>20</v>
       </c>
       <c r="I139" s="386">

</xml_diff>

<commit_message>
Added multiple violation optimisation
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DB29B7-82CD-4A8D-8CAB-AF0B2529BA04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCC2E93-E777-48F1-90B5-E99711972340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="0" windowWidth="21528" windowHeight="12360" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="236">
   <si>
     <t>week</t>
   </si>
@@ -1124,6 +1124,18 @@
   </si>
   <si>
     <t>Supplier Forecasted DEMAND</t>
+  </si>
+  <si>
+    <t>Cons</t>
+  </si>
+  <si>
+    <t>reduction can only be made to 1 supplier</t>
+  </si>
+  <si>
+    <t>Pros</t>
+  </si>
+  <si>
+    <t>multiple violations can be solved</t>
   </si>
 </sst>
 </file>
@@ -2404,7 +2416,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="23" borderId="66" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="418">
+  <cellXfs count="419">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3473,6 +3485,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -32836,10 +32851,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
-  <dimension ref="A2:AI147"/>
+  <dimension ref="A2:AI148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33003,7 +33018,9 @@
       <c r="K11" s="392">
         <v>15</v>
       </c>
-      <c r="L11" s="392"/>
+      <c r="L11" s="392">
+        <v>150</v>
+      </c>
       <c r="M11" s="392"/>
       <c r="N11" s="392"/>
       <c r="O11" s="393">
@@ -33116,7 +33133,7 @@
       </c>
       <c r="L15" s="289">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="M15" s="289">
         <f t="shared" si="0"/>
@@ -33187,19 +33204,19 @@
       </c>
       <c r="L17" s="267">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M17" s="267">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N17" s="267">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="O17" s="268">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="Q17" s="341" t="s">
         <v>48</v>
@@ -33239,7 +33256,7 @@
       </c>
       <c r="L18" s="267">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="M18" s="267">
         <f t="shared" si="3"/>
@@ -33247,11 +33264,11 @@
       </c>
       <c r="N18" s="267">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="O18" s="268">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="342" t="s">
         <v>46</v>
@@ -33282,7 +33299,7 @@
       </c>
       <c r="L19" s="267">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="M19" s="267">
         <f t="shared" si="4"/>
@@ -33294,7 +33311,7 @@
       </c>
       <c r="O19" s="268">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -33320,7 +33337,7 @@
       </c>
       <c r="J20" s="344">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="K20" s="344">
         <f t="shared" si="5"/>
@@ -33332,7 +33349,7 @@
       </c>
       <c r="M20" s="344">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N20" s="344">
         <f t="shared" si="5"/>
@@ -33413,7 +33430,7 @@
       </c>
       <c r="J22" s="313">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K22" s="313">
         <f t="shared" si="7"/>
@@ -33425,7 +33442,7 @@
       </c>
       <c r="M22" s="313">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" s="313">
         <f t="shared" si="7"/>
@@ -33459,7 +33476,7 @@
       </c>
       <c r="J23" s="373">
         <f t="shared" si="8"/>
-        <v>1200</v>
+        <v>6000</v>
       </c>
       <c r="K23" s="373">
         <f t="shared" si="8"/>
@@ -33471,7 +33488,7 @@
       </c>
       <c r="M23" s="373">
         <f t="shared" si="8"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="N23" s="373">
         <f t="shared" si="8"/>
@@ -33544,7 +33561,7 @@
       </c>
       <c r="J25" s="334">
         <f t="shared" si="9"/>
-        <v>8600</v>
+        <v>43000</v>
       </c>
       <c r="K25" s="334">
         <f t="shared" si="9"/>
@@ -33556,7 +33573,7 @@
       </c>
       <c r="M25" s="334">
         <f t="shared" si="9"/>
-        <v>4240</v>
+        <v>0</v>
       </c>
       <c r="N25" s="334">
         <f t="shared" si="9"/>
@@ -33596,7 +33613,7 @@
       </c>
       <c r="J26" s="336">
         <f t="shared" si="10"/>
-        <v>9800</v>
+        <v>49000</v>
       </c>
       <c r="K26" s="336">
         <f t="shared" si="10"/>
@@ -33608,7 +33625,7 @@
       </c>
       <c r="M26" s="336">
         <f t="shared" si="10"/>
-        <v>4840</v>
+        <v>0</v>
       </c>
       <c r="N26" s="336">
         <f t="shared" si="10"/>
@@ -33684,7 +33701,7 @@
       </c>
       <c r="J28" s="338">
         <f t="shared" si="11"/>
-        <v>16720</v>
+        <v>83600</v>
       </c>
       <c r="K28" s="338">
         <f t="shared" si="11"/>
@@ -33696,7 +33713,7 @@
       </c>
       <c r="M28" s="338">
         <f t="shared" si="11"/>
-        <v>8380</v>
+        <v>0</v>
       </c>
       <c r="N28" s="338">
         <f t="shared" si="11"/>
@@ -33733,7 +33750,7 @@
       </c>
       <c r="J29" s="292">
         <f t="shared" si="12"/>
-        <v>6920</v>
+        <v>34600</v>
       </c>
       <c r="K29" s="292">
         <f t="shared" si="12"/>
@@ -33745,7 +33762,7 @@
       </c>
       <c r="M29" s="292">
         <f t="shared" si="12"/>
-        <v>3540</v>
+        <v>0</v>
       </c>
       <c r="N29" s="292">
         <f t="shared" si="12"/>
@@ -33782,7 +33799,7 @@
       </c>
       <c r="J30" s="258">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="K30" s="258">
         <f t="shared" si="13"/>
@@ -33841,7 +33858,7 @@
       </c>
       <c r="J31" s="258">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K31" s="258">
         <f t="shared" si="14"/>
@@ -33965,7 +33982,7 @@
       </c>
       <c r="J33" s="313">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K33" s="313">
         <f t="shared" si="16"/>
@@ -34059,7 +34076,7 @@
       </c>
       <c r="J34" s="316">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="K34" s="316">
         <f t="shared" si="17"/>
@@ -34156,7 +34173,7 @@
       </c>
       <c r="J35" s="333">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>12900</v>
       </c>
       <c r="K35" s="333">
         <f t="shared" si="26"/>
@@ -34251,7 +34268,7 @@
       </c>
       <c r="J36" s="292">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>14700</v>
       </c>
       <c r="K36" s="292">
         <f t="shared" si="27"/>
@@ -34345,7 +34362,7 @@
       </c>
       <c r="J37" s="194">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>25080</v>
       </c>
       <c r="K37" s="194">
         <f t="shared" si="28"/>
@@ -34439,7 +34456,7 @@
       </c>
       <c r="J38" s="326">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>10380</v>
       </c>
       <c r="K38" s="326">
         <f t="shared" si="29"/>
@@ -34535,7 +34552,7 @@
       </c>
       <c r="J39" s="224">
         <f t="shared" si="30"/>
-        <v>6920</v>
+        <v>24220</v>
       </c>
       <c r="K39" s="224">
         <f t="shared" si="30"/>
@@ -34547,7 +34564,7 @@
       </c>
       <c r="M39" s="224">
         <f t="shared" si="30"/>
-        <v>3540</v>
+        <v>0</v>
       </c>
       <c r="N39" s="224">
         <f t="shared" si="30"/>
@@ -34628,7 +34645,7 @@
       </c>
       <c r="J40" s="330">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K40" s="330" t="e">
         <f t="shared" si="31"/>
@@ -34638,9 +34655,9 @@
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="M40" s="330">
+      <c r="M40" s="330" t="e">
         <f t="shared" si="31"/>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N40" s="330" t="e">
         <f t="shared" si="31"/>
@@ -34721,7 +34738,7 @@
       </c>
       <c r="J41" s="330">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K41" s="330" t="e">
         <f t="shared" si="32"/>
@@ -34731,9 +34748,9 @@
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="M41" s="330">
+      <c r="M41" s="330" t="e">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N41" s="330" t="e">
         <f t="shared" si="32"/>
@@ -34814,7 +34831,7 @@
       </c>
       <c r="J42" s="332">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K42" s="332" t="e">
         <f t="shared" si="33"/>
@@ -34824,9 +34841,9 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
-      <c r="M42" s="332">
+      <c r="M42" s="332" t="e">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N42" s="332" t="e">
         <f t="shared" si="33"/>
@@ -37124,7 +37141,7 @@
       </c>
       <c r="J71" s="258">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K71" s="258">
         <f t="shared" si="47"/>
@@ -37307,7 +37324,7 @@
       </c>
       <c r="J73" s="313">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K73" s="313">
         <f t="shared" si="49"/>
@@ -37397,7 +37414,7 @@
       </c>
       <c r="J74" s="316">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="K74" s="316">
         <f t="shared" si="50"/>
@@ -37490,7 +37507,7 @@
       </c>
       <c r="J75" s="194">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>3225</v>
       </c>
       <c r="K75" s="194">
         <f t="shared" si="51"/>
@@ -37581,7 +37598,7 @@
       </c>
       <c r="J76" s="292">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>3725</v>
       </c>
       <c r="K76" s="292">
         <f t="shared" si="52"/>
@@ -37629,7 +37646,7 @@
       </c>
       <c r="J77" s="194">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>6270</v>
       </c>
       <c r="K77" s="194">
         <f t="shared" si="53"/>
@@ -37677,7 +37694,7 @@
       </c>
       <c r="J78" s="326">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>2545</v>
       </c>
       <c r="K78" s="326">
         <f t="shared" si="54"/>
@@ -37727,7 +37744,7 @@
       </c>
       <c r="J79" s="224">
         <f t="shared" si="55"/>
-        <v>3560</v>
+        <v>1015</v>
       </c>
       <c r="K79" s="224">
         <f t="shared" si="55"/>
@@ -37821,7 +37838,7 @@
       </c>
       <c r="J81" s="330">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>0.77604166666666663</v>
       </c>
       <c r="K81" s="330">
         <f t="shared" si="57"/>
@@ -37878,7 +37895,7 @@
       </c>
       <c r="J82" s="332">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>0.7148876404494382</v>
       </c>
       <c r="K82" s="332">
         <f t="shared" si="58"/>
@@ -38916,7 +38933,7 @@
       </c>
       <c r="J112" s="258">
         <f t="shared" ref="J112:K112" si="74">MIN(J139,J111)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K112" s="258">
         <f t="shared" si="74"/>
@@ -39009,7 +39026,7 @@
       </c>
       <c r="J113" s="369">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K113" s="369">
         <f t="shared" si="85"/>
@@ -39103,7 +39120,7 @@
       </c>
       <c r="J115" s="316">
         <f t="shared" si="87"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="K115" s="316">
         <f t="shared" si="87"/>
@@ -39153,7 +39170,7 @@
       </c>
       <c r="J116" s="194">
         <f t="shared" si="88"/>
-        <v>0</v>
+        <v>2150</v>
       </c>
       <c r="K116" s="194">
         <f t="shared" si="88"/>
@@ -39201,7 +39218,7 @@
       </c>
       <c r="J117" s="292">
         <f t="shared" si="89"/>
-        <v>0</v>
+        <v>2270</v>
       </c>
       <c r="K117" s="292">
         <f t="shared" si="89"/>
@@ -39248,7 +39265,7 @@
       </c>
       <c r="J118" s="194">
         <f t="shared" si="90"/>
-        <v>0</v>
+        <v>4180</v>
       </c>
       <c r="K118" s="194">
         <f t="shared" si="90"/>
@@ -39295,7 +39312,7 @@
       </c>
       <c r="J119" s="326">
         <f t="shared" si="91"/>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="K119" s="326">
         <f t="shared" si="91"/>
@@ -39344,7 +39361,7 @@
       </c>
       <c r="J120" s="224">
         <f t="shared" si="92"/>
-        <v>9630</v>
+        <v>7720</v>
       </c>
       <c r="K120" s="224">
         <f t="shared" si="92"/>
@@ -39438,7 +39455,7 @@
       </c>
       <c r="J122" s="330">
         <f t="shared" si="94"/>
-        <v>0</v>
+        <v>0.20141969831410825</v>
       </c>
       <c r="K122" s="330">
         <f t="shared" si="94"/>
@@ -39495,7 +39512,7 @@
       </c>
       <c r="J123" s="332">
         <f t="shared" si="95"/>
-        <v>0</v>
+        <v>0.19833852544132918</v>
       </c>
       <c r="K123" s="332">
         <f t="shared" si="95"/>
@@ -39685,7 +39702,7 @@
       </c>
       <c r="J133" s="136">
         <f t="shared" si="96"/>
-        <v>110</v>
+        <v>270</v>
       </c>
       <c r="K133" s="136">
         <f t="shared" si="96"/>
@@ -39697,7 +39714,7 @@
       </c>
       <c r="M133" s="136">
         <f t="shared" si="96"/>
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="N133" s="136">
         <f t="shared" si="96"/>
@@ -39749,27 +39766,27 @@
       </c>
       <c r="J135" s="267">
         <f t="shared" si="97"/>
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="K135" s="267">
         <f t="shared" si="97"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L135" s="267">
         <f t="shared" si="97"/>
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="M135" s="267">
         <f t="shared" si="97"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="N135" s="267">
         <f t="shared" si="97"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="O135" s="268">
         <f t="shared" si="97"/>
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="136" spans="3:16" x14ac:dyDescent="0.3">
@@ -39795,23 +39812,23 @@
       </c>
       <c r="J136" s="267">
         <f t="shared" si="98"/>
-        <v>100</v>
+        <v>260</v>
       </c>
       <c r="K136" s="267">
         <f t="shared" si="98"/>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="L136" s="267">
         <f t="shared" si="98"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="M136" s="267">
         <f t="shared" si="98"/>
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="N136" s="267">
         <f t="shared" si="98"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O136" s="268">
         <f t="shared" si="98"/>
@@ -39841,19 +39858,19 @@
       </c>
       <c r="J137" s="267">
         <f t="shared" si="99"/>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="K137" s="267">
         <f t="shared" si="99"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="L137" s="267">
         <f t="shared" si="99"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M137" s="267">
         <f t="shared" si="99"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N137" s="267">
         <f t="shared" si="99"/>
@@ -39883,19 +39900,19 @@
       </c>
       <c r="I138" s="390">
         <f t="shared" si="100"/>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="J138" s="390">
         <f t="shared" si="100"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K138" s="390">
         <f t="shared" si="100"/>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L138" s="390">
         <f t="shared" si="100"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M138" s="390">
         <f t="shared" si="100"/>
@@ -39934,7 +39951,7 @@
       </c>
       <c r="J139" s="386">
         <f t="shared" si="101"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K139" s="386">
         <f t="shared" si="101"/>
@@ -39977,28 +39994,42 @@
       <c r="C143" s="157" t="s">
         <v>121</v>
       </c>
+      <c r="H143" s="418" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="144" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C144" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="145" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="H144" s="85" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="145" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C145" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="146" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C146" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C147" s="383" t="s">
         <v>140</v>
       </c>
       <c r="D147" s="85" t="s">
         <v>141</v>
+      </c>
+      <c r="H147" s="418" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="148" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H148" s="85" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MPS move order
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCC2E93-E777-48F1-90B5-E99711972340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09B97B9-3D2E-4C4D-8CA3-A7DADACCF8A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="37575" yWindow="1545" windowWidth="17505" windowHeight="12960" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="238">
   <si>
     <t>week</t>
   </si>
@@ -1136,6 +1136,12 @@
   </si>
   <si>
     <t>multiple violations can be solved</t>
+  </si>
+  <si>
+    <t>Amount to Move</t>
+  </si>
+  <si>
+    <t>Updated Master Production Schedule</t>
   </si>
 </sst>
 </file>
@@ -3478,6 +3484,9 @@
     <xf numFmtId="0" fontId="24" fillId="23" borderId="70" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3485,9 +3494,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7579,19 +7585,19 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="415" t="s">
+      <c r="C3" s="416" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="416"/>
-      <c r="E3" s="416"/>
-      <c r="F3" s="416"/>
-      <c r="G3" s="416"/>
-      <c r="H3" s="416"/>
-      <c r="I3" s="416"/>
-      <c r="J3" s="416"/>
-      <c r="K3" s="416"/>
-      <c r="L3" s="416"/>
-      <c r="M3" s="417"/>
+      <c r="D3" s="417"/>
+      <c r="E3" s="417"/>
+      <c r="F3" s="417"/>
+      <c r="G3" s="417"/>
+      <c r="H3" s="417"/>
+      <c r="I3" s="417"/>
+      <c r="J3" s="417"/>
+      <c r="K3" s="417"/>
+      <c r="L3" s="417"/>
+      <c r="M3" s="418"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
@@ -7963,19 +7969,19 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="415" t="s">
+      <c r="C4" s="416" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="416"/>
-      <c r="E4" s="416"/>
-      <c r="F4" s="416"/>
-      <c r="G4" s="416"/>
-      <c r="H4" s="416"/>
-      <c r="I4" s="416"/>
-      <c r="J4" s="416"/>
-      <c r="K4" s="416"/>
-      <c r="L4" s="416"/>
-      <c r="M4" s="417"/>
+      <c r="D4" s="417"/>
+      <c r="E4" s="417"/>
+      <c r="F4" s="417"/>
+      <c r="G4" s="417"/>
+      <c r="H4" s="417"/>
+      <c r="I4" s="417"/>
+      <c r="J4" s="417"/>
+      <c r="K4" s="417"/>
+      <c r="L4" s="417"/>
+      <c r="M4" s="418"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -8605,19 +8611,19 @@
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="415" t="s">
+      <c r="C23" s="416" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="416"/>
-      <c r="E23" s="416"/>
-      <c r="F23" s="416"/>
-      <c r="G23" s="416"/>
-      <c r="H23" s="416"/>
-      <c r="I23" s="416"/>
-      <c r="J23" s="416"/>
-      <c r="K23" s="416"/>
-      <c r="L23" s="416"/>
-      <c r="M23" s="417"/>
+      <c r="D23" s="417"/>
+      <c r="E23" s="417"/>
+      <c r="F23" s="417"/>
+      <c r="G23" s="417"/>
+      <c r="H23" s="417"/>
+      <c r="I23" s="417"/>
+      <c r="J23" s="417"/>
+      <c r="K23" s="417"/>
+      <c r="L23" s="417"/>
+      <c r="M23" s="418"/>
       <c r="O23" s="24" t="s">
         <v>68</v>
       </c>
@@ -10660,17 +10666,17 @@
       <c r="C51" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="416" t="s">
+      <c r="D51" s="417" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="416"/>
-      <c r="F51" s="416"/>
-      <c r="G51" s="416"/>
-      <c r="H51" s="416"/>
-      <c r="I51" s="416"/>
-      <c r="J51" s="416"/>
-      <c r="K51" s="416"/>
-      <c r="L51" s="417"/>
+      <c r="E51" s="417"/>
+      <c r="F51" s="417"/>
+      <c r="G51" s="417"/>
+      <c r="H51" s="417"/>
+      <c r="I51" s="417"/>
+      <c r="J51" s="417"/>
+      <c r="K51" s="417"/>
+      <c r="L51" s="418"/>
       <c r="M51"/>
       <c r="N51"/>
       <c r="O51"/>
@@ -32851,10 +32857,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
-  <dimension ref="A2:AI148"/>
+  <dimension ref="A2:AI150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView tabSelected="1" topLeftCell="C124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39611,7 +39617,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D129" s="118" t="s">
         <v>33</v>
       </c>
@@ -39625,7 +39631,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="130" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D130" s="118" t="s">
         <v>35</v>
       </c>
@@ -39636,7 +39642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D131" s="118" t="s">
         <v>224</v>
       </c>
@@ -39644,7 +39650,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="132" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E132" s="71" t="s">
         <v>96</v>
       </c>
@@ -39679,7 +39685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D133" s="129" t="s">
         <v>231</v>
       </c>
@@ -39725,7 +39731,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D134" s="130" t="s">
         <v>114</v>
       </c>
@@ -39741,7 +39747,7 @@
       <c r="N134" s="96"/>
       <c r="O134" s="107"/>
     </row>
-    <row r="135" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D135" s="131" t="s">
         <v>85</v>
       </c>
@@ -39789,7 +39795,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D136" s="131" t="s">
         <v>30</v>
       </c>
@@ -39835,7 +39841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D137" s="132" t="s">
         <v>113</v>
       </c>
@@ -39881,7 +39887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D138" s="133" t="s">
         <v>225</v>
       </c>
@@ -39928,7 +39934,7 @@
       </c>
       <c r="P138" s="177"/>
     </row>
-    <row r="139" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D139" s="384" t="s">
         <v>223</v>
       </c>
@@ -39938,7 +39944,7 @@
         <v>0</v>
       </c>
       <c r="G139" s="386">
-        <f t="shared" ref="G139:O139" si="101">IF(G136&gt;$E$131,G136-$E$131,0)</f>
+        <f t="shared" ref="G139:O140" si="101">IF(G136&gt;$E$131,G136-$E$131,0)</f>
         <v>0</v>
       </c>
       <c r="H139" s="386">
@@ -39975,60 +39981,154 @@
       </c>
       <c r="P139" s="177"/>
     </row>
-    <row r="140" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="H140" s="382"/>
-      <c r="I140" s="381"/>
-    </row>
-    <row r="141" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="H141" s="412">
+    <row r="140" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D140" s="384" t="s">
+        <v>236</v>
+      </c>
+      <c r="E140" s="385"/>
+      <c r="F140" s="386">
+        <f>IF(F137&gt;$E$131,F137-$E$131,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G140" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="H140" s="386">
+        <f>IF(H137&gt;$E$131,H137-$E$131,0)</f>
+        <v>50</v>
+      </c>
+      <c r="I140" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="J140" s="386">
+        <f t="shared" si="101"/>
+        <v>100</v>
+      </c>
+      <c r="K140" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="L140" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="M140" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="N140" s="386">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="O140" s="387">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="P140" s="177"/>
+    </row>
+    <row r="141" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D141" s="132" t="s">
+        <v>237</v>
+      </c>
+      <c r="E141" s="266"/>
+      <c r="F141" s="267">
+        <f>F137-F140</f>
+        <v>0</v>
+      </c>
+      <c r="G141" s="267">
+        <f>IF(G137&lt;$E$131, G137-G140)</f>
+        <v>100</v>
+      </c>
+      <c r="H141" s="267">
+        <f t="shared" ref="G141:O141" si="102">H137-H140</f>
+        <v>200</v>
+      </c>
+      <c r="I141" s="267">
+        <f t="shared" si="102"/>
+        <v>150</v>
+      </c>
+      <c r="J141" s="267">
+        <f t="shared" si="102"/>
+        <v>200</v>
+      </c>
+      <c r="K141" s="267">
+        <f t="shared" si="102"/>
+        <v>50</v>
+      </c>
+      <c r="L141" s="267">
+        <f t="shared" si="102"/>
+        <v>100</v>
+      </c>
+      <c r="M141" s="267">
+        <f t="shared" si="102"/>
+        <v>50</v>
+      </c>
+      <c r="N141" s="267">
+        <f t="shared" si="102"/>
+        <v>50</v>
+      </c>
+      <c r="O141" s="267">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+      <c r="P141" s="177"/>
+    </row>
+    <row r="142" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H142" s="382"/>
+      <c r="I142" s="381"/>
+    </row>
+    <row r="143" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H143" s="412">
         <f>MIN(H119,H78,H38)</f>
         <v>2755</v>
       </c>
-      <c r="I141" s="381"/>
-    </row>
-    <row r="142" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="H142" s="382"/>
-      <c r="I142" s="381"/>
-    </row>
-    <row r="143" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C143" s="157" t="s">
+      <c r="I143" s="381"/>
+    </row>
+    <row r="144" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="H144" s="382"/>
+      <c r="I144" s="381"/>
+    </row>
+    <row r="145" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C145" s="157" t="s">
         <v>121</v>
       </c>
-      <c r="H143" s="418" t="s">
+      <c r="H145" s="415" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="144" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C144" t="s">
-        <v>137</v>
-      </c>
-      <c r="H144" s="85" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="145" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C145" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="146" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C146" t="s">
+        <v>137</v>
+      </c>
+      <c r="H146" s="85" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="147" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C147" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="148" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C148" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C147" s="383" t="s">
+    <row r="149" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C149" s="383" t="s">
         <v>140</v>
       </c>
-      <c r="D147" s="85" t="s">
+      <c r="D149" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="H147" s="418" t="s">
+      <c r="H149" s="415" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="148" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H148" s="85" t="s">
+    <row r="150" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H150" s="85" t="s">
         <v>233</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added updated spot forecast demand
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09B97B9-3D2E-4C4D-8CA3-A7DADACCF8A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2896093A-5D71-4806-B5D9-B8DE0BE4D6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37575" yWindow="1545" windowWidth="17505" windowHeight="12960" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="28680" yWindow="240" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32859,8 +32859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
   <dimension ref="A2:AI150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H127" sqref="H127"/>
+    <sheetView tabSelected="1" topLeftCell="D117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O149" sqref="O149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40042,7 +40042,7 @@
         <v>100</v>
       </c>
       <c r="H141" s="267">
-        <f t="shared" ref="G141:O141" si="102">H137-H140</f>
+        <f t="shared" ref="H141:O141" si="102">H137-H140</f>
         <v>200</v>
       </c>
       <c r="I141" s="267">

</xml_diff>

<commit_message>
solved 3 MPS violation
</commit_message>
<xml_diff>
--- a/DRP/DRP.xlsx
+++ b/DRP/DRP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2896093A-5D71-4806-B5D9-B8DE0BE4D6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4C398B-22F9-4BA6-AF4E-440331010DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="240" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="3" activeTab="8" xr2:uid="{EC6B9FCF-015A-4253-A96B-EFFF1F70826F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="239">
   <si>
     <t>week</t>
   </si>
@@ -1141,7 +1141,10 @@
     <t>Amount to Move</t>
   </si>
   <si>
-    <t>Updated Master Production Schedule</t>
+    <t>Supply Lot Size</t>
+  </si>
+  <si>
+    <t>Delivery Lead Time</t>
   </si>
 </sst>
 </file>
@@ -17780,7 +17783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8A3298-59F5-4F80-A43A-018CB86A5248}">
   <dimension ref="A2:AU168"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AH49" sqref="AH49"/>
     </sheetView>
   </sheetViews>
@@ -32857,10 +32860,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47FF7E8-2777-4C95-B865-13763CE79903}">
-  <dimension ref="A2:AI150"/>
+  <dimension ref="A2:AI149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O149" sqref="O149"/>
+    <sheetView tabSelected="1" topLeftCell="D118" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32935,7 +32938,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D7" s="118" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="E7" s="120">
         <v>2</v>
@@ -32946,7 +32949,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D8" s="118" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
       <c r="E8" s="121">
         <v>20</v>
@@ -35148,7 +35151,7 @@
     </row>
     <row r="47" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D47" s="118" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="E47" s="120">
         <v>1</v>
@@ -35208,7 +35211,7 @@
     </row>
     <row r="48" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D48" s="118" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
       <c r="E48" s="122">
         <v>20</v>
@@ -35421,7 +35424,9 @@
       <c r="E51" s="276"/>
       <c r="F51" s="392"/>
       <c r="G51" s="392"/>
-      <c r="H51" s="392"/>
+      <c r="H51" s="392">
+        <v>0</v>
+      </c>
       <c r="I51" s="406">
         <v>20</v>
       </c>
@@ -38010,7 +38015,7 @@
     </row>
     <row r="88" spans="3:35" x14ac:dyDescent="0.3">
       <c r="D88" s="118" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="E88" s="120">
         <v>0</v>
@@ -38024,7 +38029,7 @@
     </row>
     <row r="89" spans="3:35" x14ac:dyDescent="0.3">
       <c r="D89" s="118" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
       <c r="E89" s="122">
         <v>10</v>
@@ -38094,7 +38099,9 @@
       </c>
       <c r="E92" s="276"/>
       <c r="F92" s="413"/>
-      <c r="G92" s="413"/>
+      <c r="G92" s="413">
+        <v>0</v>
+      </c>
       <c r="H92" s="413">
         <v>15</v>
       </c>
@@ -39617,7 +39624,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D129" s="118" t="s">
         <v>33</v>
       </c>
@@ -39631,7 +39638,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="130" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D130" s="118" t="s">
         <v>35</v>
       </c>
@@ -39642,7 +39649,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D131" s="118" t="s">
         <v>224</v>
       </c>
@@ -39650,7 +39657,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="132" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E132" s="71" t="s">
         <v>96</v>
       </c>
@@ -39685,7 +39692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D133" s="129" t="s">
         <v>231</v>
       </c>
@@ -39699,7 +39706,7 @@
         <v>80</v>
       </c>
       <c r="H133" s="136">
-        <f t="shared" si="96"/>
+        <f>SUM(H101,H60,H20)</f>
         <v>240</v>
       </c>
       <c r="I133" s="136">
@@ -39731,7 +39738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D134" s="130" t="s">
         <v>114</v>
       </c>
@@ -39747,7 +39754,7 @@
       <c r="N134" s="96"/>
       <c r="O134" s="107"/>
     </row>
-    <row r="135" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D135" s="131" t="s">
         <v>85</v>
       </c>
@@ -39795,7 +39802,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D136" s="131" t="s">
         <v>30</v>
       </c>
@@ -39841,7 +39848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D137" s="132" t="s">
         <v>113</v>
       </c>
@@ -39887,7 +39894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D138" s="133" t="s">
         <v>225</v>
       </c>
@@ -39934,7 +39941,7 @@
       </c>
       <c r="P138" s="177"/>
     </row>
-    <row r="139" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D139" s="384" t="s">
         <v>223</v>
       </c>
@@ -39981,7 +39988,7 @@
       </c>
       <c r="P139" s="177"/>
     </row>
-    <row r="140" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D140" s="384" t="s">
         <v>236</v>
       </c>
@@ -40028,107 +40035,60 @@
       </c>
       <c r="P140" s="177"/>
     </row>
-    <row r="141" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D141" s="132" t="s">
-        <v>237</v>
-      </c>
-      <c r="E141" s="266"/>
-      <c r="F141" s="267">
-        <f>F137-F140</f>
-        <v>0</v>
-      </c>
-      <c r="G141" s="267">
-        <f>IF(G137&lt;$E$131, G137-G140)</f>
-        <v>100</v>
-      </c>
-      <c r="H141" s="267">
-        <f t="shared" ref="H141:O141" si="102">H137-H140</f>
-        <v>200</v>
-      </c>
-      <c r="I141" s="267">
-        <f t="shared" si="102"/>
-        <v>150</v>
-      </c>
-      <c r="J141" s="267">
-        <f t="shared" si="102"/>
-        <v>200</v>
-      </c>
-      <c r="K141" s="267">
-        <f t="shared" si="102"/>
-        <v>50</v>
-      </c>
-      <c r="L141" s="267">
-        <f t="shared" si="102"/>
-        <v>100</v>
-      </c>
-      <c r="M141" s="267">
-        <f t="shared" si="102"/>
-        <v>50</v>
-      </c>
-      <c r="N141" s="267">
-        <f t="shared" si="102"/>
-        <v>50</v>
-      </c>
-      <c r="O141" s="267">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="P141" s="177"/>
-    </row>
-    <row r="142" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="H142" s="382"/>
-      <c r="I142" s="381"/>
-    </row>
-    <row r="143" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="H143" s="412">
+    <row r="141" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="H141" s="382"/>
+      <c r="I141" s="381"/>
+    </row>
+    <row r="142" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="H142" s="412">
         <f>MIN(H119,H78,H38)</f>
         <v>2755</v>
       </c>
+      <c r="I142" s="381"/>
+    </row>
+    <row r="143" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="H143" s="382"/>
       <c r="I143" s="381"/>
     </row>
-    <row r="144" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="H144" s="382"/>
-      <c r="I144" s="381"/>
+    <row r="144" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C144" s="157" t="s">
+        <v>121</v>
+      </c>
+      <c r="H144" s="415" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="145" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C145" s="157" t="s">
-        <v>121</v>
-      </c>
-      <c r="H145" s="415" t="s">
-        <v>234</v>
+      <c r="C145" t="s">
+        <v>137</v>
+      </c>
+      <c r="H145" s="85" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="146" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C146" t="s">
-        <v>137</v>
-      </c>
-      <c r="H146" s="85" t="s">
-        <v>235</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C147" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
     </row>
     <row r="148" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C148" t="s">
-        <v>156</v>
+      <c r="C148" s="383" t="s">
+        <v>140</v>
+      </c>
+      <c r="D148" s="85" t="s">
+        <v>141</v>
+      </c>
+      <c r="H148" s="415" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="149" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C149" s="383" t="s">
-        <v>140</v>
-      </c>
-      <c r="D149" s="85" t="s">
-        <v>141</v>
-      </c>
-      <c r="H149" s="415" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="150" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="H150" s="85" t="s">
+      <c r="H149" s="85" t="s">
         <v>233</v>
       </c>
     </row>

</xml_diff>